<commit_message>
[ADDS] Plastica order document [CHANGE] Mapping of UDF
</commit_message>
<xml_diff>
--- a/TransusFieldsMapping.xlsx
+++ b/TransusFieldsMapping.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1430" uniqueCount="441">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1444" uniqueCount="451">
   <si>
     <t>Table</t>
   </si>
@@ -1338,6 +1338,36 @@
   </si>
   <si>
     <t>Kleursysteem</t>
+  </si>
+  <si>
+    <t>CRD1</t>
+  </si>
+  <si>
+    <t>OCDR</t>
+  </si>
+  <si>
+    <t>BarCode</t>
+  </si>
+  <si>
+    <t>Bar code</t>
+  </si>
+  <si>
+    <t>PartnerGLN</t>
+  </si>
+  <si>
+    <t>GLN de partner</t>
+  </si>
+  <si>
+    <t>GLN adres</t>
+  </si>
+  <si>
+    <t>AddressGLN</t>
+  </si>
+  <si>
+    <t>AddressGLN -&gt; billing to</t>
+  </si>
+  <si>
+    <t>AddressGLN -&gt; shipping to</t>
   </si>
 </sst>
 </file>
@@ -1490,7 +1520,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1544,6 +1574,8 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="40% - Accent4" xfId="4" builtinId="43"/>
@@ -1766,13 +1798,6 @@
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
@@ -1981,6 +2006,13 @@
         <right/>
         <top/>
         <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -2227,11 +2259,11 @@
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table3713" displayName="Table3713" ref="L101:P115" headerRowCount="0" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
   <tableColumns count="5">
-    <tableColumn id="1" name="Column1" headerRowDxfId="4" dataCellStyle="Normal"/>
-    <tableColumn id="2" name="Column2" headerRowDxfId="3" dataCellStyle="Normal"/>
-    <tableColumn id="3" name="Column3" headerRowDxfId="2" dataCellStyle="Normal"/>
-    <tableColumn id="4" name="Column4" headerRowDxfId="1" dataCellStyle="Normal"/>
-    <tableColumn id="5" name="Column5" headerRowDxfId="0" dataCellStyle="Normal"/>
+    <tableColumn id="1" name="Column1" headerRowDxfId="14" dataCellStyle="Normal"/>
+    <tableColumn id="2" name="Column2" headerRowDxfId="13" dataCellStyle="Normal"/>
+    <tableColumn id="3" name="Column3" headerRowDxfId="12" dataCellStyle="Normal"/>
+    <tableColumn id="4" name="Column4" headerRowDxfId="11" dataCellStyle="Normal"/>
+    <tableColumn id="5" name="Column5" headerRowDxfId="10" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2273,26 +2305,26 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table22" displayName="Table22" ref="B5:F41" headerRowCount="0" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table22" displayName="Table22" ref="B5:F44" headerRowCount="0" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
   <tableColumns count="5">
-    <tableColumn id="1" name="Column1" headerRowDxfId="20" dataCellStyle="Normal"/>
-    <tableColumn id="2" name="Column2" headerRowDxfId="19" dataCellStyle="Normal"/>
-    <tableColumn id="3" name="Column3" headerRowDxfId="18" dataCellStyle="Normal"/>
-    <tableColumn id="4" name="Column4" headerRowDxfId="17" dataCellStyle="Normal"/>
-    <tableColumn id="5" name="Column5" headerRowDxfId="16" dataCellStyle="Normal"/>
+    <tableColumn id="1" name="Column1" headerRowDxfId="9" dataCellStyle="Normal"/>
+    <tableColumn id="2" name="Column2" headerRowDxfId="8" dataCellStyle="Normal"/>
+    <tableColumn id="3" name="Column3" headerRowDxfId="7" dataCellStyle="Normal"/>
+    <tableColumn id="4" name="Column4" headerRowDxfId="6" dataCellStyle="Normal"/>
+    <tableColumn id="5" name="Column5" headerRowDxfId="5" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table37" displayName="Table37" ref="B43:F55" headerRowCount="0" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table37" displayName="Table37" ref="B46:F59" headerRowCount="0" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
   <tableColumns count="5">
-    <tableColumn id="1" name="Column1" headerRowDxfId="15" dataCellStyle="Normal"/>
-    <tableColumn id="2" name="Column2" headerRowDxfId="14" dataCellStyle="Normal"/>
-    <tableColumn id="3" name="Column3" headerRowDxfId="13" dataCellStyle="Normal"/>
-    <tableColumn id="4" name="Column4" headerRowDxfId="12" dataCellStyle="Normal"/>
-    <tableColumn id="5" name="Column5" headerRowDxfId="11" dataCellStyle="Normal"/>
+    <tableColumn id="1" name="Column1" headerRowDxfId="4" dataCellStyle="Normal"/>
+    <tableColumn id="2" name="Column2" headerRowDxfId="3" dataCellStyle="Normal"/>
+    <tableColumn id="3" name="Column3" headerRowDxfId="2" dataCellStyle="Normal"/>
+    <tableColumn id="4" name="Column4" headerRowDxfId="1" dataCellStyle="Normal"/>
+    <tableColumn id="5" name="Column5" headerRowDxfId="0" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2310,7 +2342,7 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table59" displayName="Table59" ref="H5:J41" headerRowCount="0" totalsRowShown="0" tableBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table59" displayName="Table59" ref="H5:J41" headerRowCount="0" totalsRowShown="0" tableBorderDxfId="20">
   <tableColumns count="3">
     <tableColumn id="1" name="Column1"/>
     <tableColumn id="2" name="Column2"/>
@@ -2323,11 +2355,11 @@
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table2212" displayName="Table2212" ref="L5:P99" headerRowCount="0" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
   <tableColumns count="5">
-    <tableColumn id="1" name="Column1" headerRowDxfId="9" dataCellStyle="Normal"/>
-    <tableColumn id="2" name="Column2" headerRowDxfId="8" dataCellStyle="Normal"/>
-    <tableColumn id="3" name="Column3" headerRowDxfId="7" dataCellStyle="Normal"/>
-    <tableColumn id="4" name="Column4" headerRowDxfId="6" dataCellStyle="Normal"/>
-    <tableColumn id="5" name="Column5" headerRowDxfId="5" dataCellStyle="Normal"/>
+    <tableColumn id="1" name="Column1" headerRowDxfId="19" dataCellStyle="Normal"/>
+    <tableColumn id="2" name="Column2" headerRowDxfId="18" dataCellStyle="Normal"/>
+    <tableColumn id="3" name="Column3" headerRowDxfId="17" dataCellStyle="Normal"/>
+    <tableColumn id="4" name="Column4" headerRowDxfId="16" dataCellStyle="Normal"/>
+    <tableColumn id="5" name="Column5" headerRowDxfId="15" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2622,8 +2654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J116"/>
   <sheetViews>
-    <sheetView topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="F114" sqref="F114"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5648,8 +5680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P115"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G45" sqref="G45"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5659,7 +5691,7 @@
     <col min="3" max="3" width="25.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31.7109375" customWidth="1"/>
     <col min="5" max="5" width="11" style="14" customWidth="1"/>
-    <col min="6" max="6" width="24.42578125" customWidth="1"/>
+    <col min="6" max="6" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.140625" customWidth="1"/>
     <col min="8" max="8" width="31.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="31.7109375" style="2" bestFit="1" customWidth="1"/>
@@ -5987,7 +6019,7 @@
         <v>125</v>
       </c>
       <c r="E10">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F10" t="str">
         <f>Table59[[#This Row],[Column1]]</f>
@@ -6489,7 +6521,7 @@
         <v>25</v>
       </c>
       <c r="I22" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="J22"/>
       <c r="L22" t="s">
@@ -6909,7 +6941,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>277</v>
       </c>
@@ -6949,7 +6981,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>277</v>
       </c>
@@ -6989,7 +7021,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>277</v>
       </c>
@@ -7029,7 +7061,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="36" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>277</v>
       </c>
@@ -7069,7 +7101,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="37" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>277</v>
       </c>
@@ -7109,7 +7141,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="38" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>277</v>
       </c>
@@ -7149,7 +7181,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="39" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>277</v>
       </c>
@@ -7189,7 +7221,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="40" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>277</v>
       </c>
@@ -7231,7 +7263,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="41" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>277</v>
       </c>
@@ -7273,14 +7305,26 @@
         <v>429</v>
       </c>
     </row>
-    <row r="42" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B42" s="9" t="s">
-        <v>427</v>
-      </c>
-      <c r="C42" s="10"/>
-      <c r="D42" s="10"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="10"/>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>449</v>
+      </c>
+      <c r="B42" s="23" t="s">
+        <v>441</v>
+      </c>
+      <c r="C42" s="23" t="s">
+        <v>448</v>
+      </c>
+      <c r="D42" s="23" t="s">
+        <v>447</v>
+      </c>
+      <c r="E42" s="23">
+        <v>13</v>
+      </c>
+      <c r="F42" s="24" t="str">
+        <f>H26</f>
+        <v>InvoiceeGLN</v>
+      </c>
       <c r="H42" s="15" t="s">
         <v>427</v>
       </c>
@@ -7302,22 +7346,25 @@
         <v>429</v>
       </c>
     </row>
-    <row r="43" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
-        <v>321</v>
-      </c>
-      <c r="C43" t="s">
-        <v>82</v>
-      </c>
-      <c r="D43" t="s">
-        <v>188</v>
-      </c>
-      <c r="E43">
-        <v>6</v>
-      </c>
-      <c r="F43" t="str">
-        <f>Table48[[#This Row],[Column1]]</f>
-        <v>LineNumber</v>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>450</v>
+      </c>
+      <c r="B43" s="23" t="s">
+        <v>441</v>
+      </c>
+      <c r="C43" s="23" t="s">
+        <v>448</v>
+      </c>
+      <c r="D43" s="23" t="s">
+        <v>447</v>
+      </c>
+      <c r="E43" s="23">
+        <v>13</v>
+      </c>
+      <c r="F43" s="24" t="str">
+        <f>CONCATENATE(H28, " or ", H20)</f>
+        <v>DeliveryPartyGLN or BuyerGLN</v>
       </c>
       <c r="H43" t="s">
         <v>82</v>
@@ -7342,22 +7389,22 @@
         <v>429</v>
       </c>
     </row>
-    <row r="44" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
-        <v>321</v>
-      </c>
-      <c r="C44" t="s">
-        <v>85</v>
-      </c>
-      <c r="D44" t="s">
-        <v>191</v>
-      </c>
-      <c r="E44">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B44" s="23" t="s">
+        <v>442</v>
+      </c>
+      <c r="C44" s="23" t="s">
+        <v>445</v>
+      </c>
+      <c r="D44" s="23" t="s">
+        <v>446</v>
+      </c>
+      <c r="E44" s="23">
         <v>13</v>
       </c>
-      <c r="F44" t="str">
-        <f>Table48[[#This Row],[Column1]]</f>
-        <v>GTIN</v>
+      <c r="F44" s="24" t="str">
+        <f>H20</f>
+        <v>BuyerGLN</v>
       </c>
       <c r="H44" t="s">
         <v>85</v>
@@ -7382,23 +7429,14 @@
         <v>429</v>
       </c>
     </row>
-    <row r="45" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
-        <v>321</v>
-      </c>
-      <c r="C45" t="s">
-        <v>84</v>
-      </c>
-      <c r="D45" t="s">
-        <v>190</v>
-      </c>
-      <c r="E45">
-        <v>35</v>
-      </c>
-      <c r="F45" t="str">
-        <f>Table48[[#This Row],[Column1]]</f>
-        <v>ArticleCodeSupplier</v>
-      </c>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B45" s="9" t="s">
+        <v>427</v>
+      </c>
+      <c r="C45" s="10"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="10"/>
       <c r="H45" t="s">
         <v>84</v>
       </c>
@@ -7422,22 +7460,22 @@
         <v>429</v>
       </c>
     </row>
-    <row r="46" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
-        <v>321</v>
-      </c>
-      <c r="C46" t="s">
-        <v>87</v>
-      </c>
-      <c r="D46" t="s">
-        <v>193</v>
-      </c>
-      <c r="E46">
-        <v>10</v>
-      </c>
-      <c r="F46" t="str">
-        <f>Table48[[#This Row],[Column1]]</f>
-        <v>OrderedQuantity</v>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B46" s="23" t="s">
+        <v>275</v>
+      </c>
+      <c r="C46" s="23" t="s">
+        <v>443</v>
+      </c>
+      <c r="D46" s="23" t="s">
+        <v>444</v>
+      </c>
+      <c r="E46" s="23">
+        <v>13</v>
+      </c>
+      <c r="F46" s="24" t="str">
+        <f>H44</f>
+        <v>GTIN</v>
       </c>
       <c r="H46" t="s">
         <v>87</v>
@@ -7464,22 +7502,22 @@
         <v>429</v>
       </c>
     </row>
-    <row r="47" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>321</v>
       </c>
       <c r="C47" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D47" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="E47">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="F47" t="str">
-        <f>Table48[[#This Row],[Column1]]</f>
-        <v>ColourCode</v>
+        <f>H43</f>
+        <v>LineNumber</v>
       </c>
       <c r="H47" t="s">
         <v>89</v>
@@ -7504,22 +7542,22 @@
         <v>429</v>
       </c>
     </row>
-    <row r="48" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>321</v>
       </c>
       <c r="C48" t="s">
-        <v>439</v>
+        <v>85</v>
       </c>
       <c r="D48" t="s">
-        <v>440</v>
+        <v>191</v>
       </c>
       <c r="E48">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="F48" t="str">
-        <f>Table48[[#This Row],[Column1]]</f>
-        <v>ColourSystem</v>
+        <f>H44</f>
+        <v>GTIN</v>
       </c>
       <c r="H48" t="s">
         <v>439</v>
@@ -7549,17 +7587,17 @@
         <v>321</v>
       </c>
       <c r="C49" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D49" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="E49">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="F49" t="str">
-        <f>Table48[[#This Row],[Column1]]</f>
-        <v>Length</v>
+        <f>H45</f>
+        <v>ArticleCodeSupplier</v>
       </c>
       <c r="H49" t="s">
         <v>90</v>
@@ -7589,17 +7627,17 @@
         <v>321</v>
       </c>
       <c r="C50" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D50" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="E50">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F50" t="str">
-        <f>Table48[[#This Row],[Column1]]</f>
-        <v>LengthUnitCode</v>
+        <f>H46</f>
+        <v>OrderedQuantity</v>
       </c>
       <c r="H50" t="s">
         <v>91</v>
@@ -7629,17 +7667,17 @@
         <v>321</v>
       </c>
       <c r="C51" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D51" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E51">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="F51" t="str">
-        <f>Table48[[#This Row],[Column1]]</f>
-        <v>Width</v>
+        <f>H47</f>
+        <v>ColourCode</v>
       </c>
       <c r="H51" t="s">
         <v>92</v>
@@ -7669,17 +7707,17 @@
         <v>321</v>
       </c>
       <c r="C52" t="s">
-        <v>93</v>
+        <v>439</v>
       </c>
       <c r="D52" t="s">
-        <v>199</v>
+        <v>440</v>
       </c>
       <c r="E52">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="F52" t="str">
-        <f>Table48[[#This Row],[Column1]]</f>
-        <v>WidthUnitCode</v>
+        <f>H48</f>
+        <v>ColourSystem</v>
       </c>
       <c r="H52" t="s">
         <v>93</v>
@@ -7709,17 +7747,17 @@
         <v>321</v>
       </c>
       <c r="C53" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D53" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="E53">
         <v>20</v>
       </c>
       <c r="F53" t="str">
-        <f>Table48[[#This Row],[Column1]]</f>
-        <v>Height</v>
+        <f>H49</f>
+        <v>Length</v>
       </c>
       <c r="H53" t="s">
         <v>94</v>
@@ -7749,17 +7787,17 @@
         <v>321</v>
       </c>
       <c r="C54" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D54" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="E54">
         <v>4</v>
       </c>
       <c r="F54" t="str">
-        <f>Table48[[#This Row],[Column1]]</f>
-        <v>HeightUnitCode</v>
+        <f>H50</f>
+        <v>LengthUnitCode</v>
       </c>
       <c r="H54" t="s">
         <v>95</v>
@@ -7790,17 +7828,17 @@
         <v>321</v>
       </c>
       <c r="C55" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D55" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="E55">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="F55" t="str">
-        <f>Table48[[#This Row],[Column1]]</f>
-        <v>RetailPrice</v>
+        <f>H51</f>
+        <v>Width</v>
       </c>
       <c r="H55" t="s">
         <v>96</v>
@@ -7828,6 +7866,22 @@
       </c>
     </row>
     <row r="56" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>321</v>
+      </c>
+      <c r="C56" t="s">
+        <v>93</v>
+      </c>
+      <c r="D56" t="s">
+        <v>199</v>
+      </c>
+      <c r="E56">
+        <v>4</v>
+      </c>
+      <c r="F56" t="str">
+        <f>H52</f>
+        <v>WidthUnitCode</v>
+      </c>
       <c r="L56" t="s">
         <v>277</v>
       </c>
@@ -7846,6 +7900,22 @@
       </c>
     </row>
     <row r="57" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>321</v>
+      </c>
+      <c r="C57" t="s">
+        <v>94</v>
+      </c>
+      <c r="D57" t="s">
+        <v>200</v>
+      </c>
+      <c r="E57">
+        <v>20</v>
+      </c>
+      <c r="F57" t="str">
+        <f>H53</f>
+        <v>Height</v>
+      </c>
       <c r="L57" t="s">
         <v>277</v>
       </c>
@@ -7864,6 +7934,22 @@
       </c>
     </row>
     <row r="58" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>321</v>
+      </c>
+      <c r="C58" t="s">
+        <v>95</v>
+      </c>
+      <c r="D58" t="s">
+        <v>201</v>
+      </c>
+      <c r="E58">
+        <v>4</v>
+      </c>
+      <c r="F58" t="str">
+        <f>H54</f>
+        <v>HeightUnitCode</v>
+      </c>
       <c r="L58" t="s">
         <v>277</v>
       </c>
@@ -7882,6 +7968,22 @@
       </c>
     </row>
     <row r="59" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>321</v>
+      </c>
+      <c r="C59" t="s">
+        <v>96</v>
+      </c>
+      <c r="D59" t="s">
+        <v>202</v>
+      </c>
+      <c r="E59">
+        <v>12</v>
+      </c>
+      <c r="F59" t="str">
+        <f>H55</f>
+        <v>RetailPrice</v>
+      </c>
       <c r="L59" t="s">
         <v>277</v>
       </c>

</xml_diff>

<commit_message>
[CHANGE] Target framework to .NET 4.5.2
</commit_message>
<xml_diff>
--- a/TransusFieldsMapping.xlsx
+++ b/TransusFieldsMapping.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Order Plastica v2" sheetId="1" r:id="rId1"/>
     <sheet name="Order Veris -&gt; Plastica bericht" sheetId="2" r:id="rId2"/>
+    <sheet name="Order Galvano - &gt; Plastica beri" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1444" uniqueCount="451">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2149" uniqueCount="451">
   <si>
     <t>Table</t>
   </si>
@@ -1355,9 +1356,6 @@
     <t>PartnerGLN</t>
   </si>
   <si>
-    <t>GLN de partner</t>
-  </si>
-  <si>
     <t>GLN adres</t>
   </si>
   <si>
@@ -1368,6 +1366,9 @@
   </si>
   <si>
     <t>AddressGLN -&gt; shipping to</t>
+  </si>
+  <si>
+    <t>GLN van de partner</t>
   </si>
 </sst>
 </file>
@@ -1585,7 +1586,436 @@
     <cellStyle name="Input" xfId="2" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="32">
+  <dxfs count="53">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="8" tint="0.59999389629810485"/>
+          <bgColor theme="8" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="8" tint="0.59999389629810485"/>
+          <bgColor theme="8" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="8" tint="0.59999389629810485"/>
+          <bgColor theme="8" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="8" tint="0.59999389629810485"/>
+          <bgColor theme="8" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="8" tint="0.59999389629810485"/>
+          <bgColor theme="8" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="8" tint="0.59999389629810485"/>
+          <bgColor theme="8" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="8" tint="0.59999389629810485"/>
+          <bgColor theme="8" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="8" tint="0.59999389629810485"/>
+          <bgColor theme="8" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="8" tint="0.59999389629810485"/>
+          <bgColor theme="8" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="8" tint="0.59999389629810485"/>
+          <bgColor theme="8" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
@@ -2246,11 +2676,11 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B5:F100" headerRowCount="0" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
   <tableColumns count="5">
-    <tableColumn id="1" name="Column1" headerRowDxfId="31" dataCellStyle="Normal"/>
-    <tableColumn id="2" name="Column2" headerRowDxfId="30" dataCellStyle="Normal"/>
-    <tableColumn id="3" name="Column3" headerRowDxfId="29" dataCellStyle="Normal"/>
-    <tableColumn id="4" name="Column4" headerRowDxfId="28" dataCellStyle="Normal"/>
-    <tableColumn id="5" name="Column5" headerRowDxfId="27" dataCellStyle="Normal"/>
+    <tableColumn id="1" name="Column1" headerRowDxfId="52" dataCellStyle="Normal"/>
+    <tableColumn id="2" name="Column2" headerRowDxfId="51" dataCellStyle="Normal"/>
+    <tableColumn id="3" name="Column3" headerRowDxfId="50" dataCellStyle="Normal"/>
+    <tableColumn id="4" name="Column4" headerRowDxfId="49" dataCellStyle="Normal"/>
+    <tableColumn id="5" name="Column5" headerRowDxfId="48" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2259,11 +2689,85 @@
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table3713" displayName="Table3713" ref="L101:P115" headerRowCount="0" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
   <tableColumns count="5">
-    <tableColumn id="1" name="Column1" headerRowDxfId="14" dataCellStyle="Normal"/>
-    <tableColumn id="2" name="Column2" headerRowDxfId="13" dataCellStyle="Normal"/>
-    <tableColumn id="3" name="Column3" headerRowDxfId="12" dataCellStyle="Normal"/>
-    <tableColumn id="4" name="Column4" headerRowDxfId="11" dataCellStyle="Normal"/>
-    <tableColumn id="5" name="Column5" headerRowDxfId="10" dataCellStyle="Normal"/>
+    <tableColumn id="1" name="Column1" headerRowDxfId="35" dataCellStyle="Normal"/>
+    <tableColumn id="2" name="Column2" headerRowDxfId="34" dataCellStyle="Normal"/>
+    <tableColumn id="3" name="Column3" headerRowDxfId="33" dataCellStyle="Normal"/>
+    <tableColumn id="4" name="Column4" headerRowDxfId="32" dataCellStyle="Normal"/>
+    <tableColumn id="5" name="Column5" headerRowDxfId="31" dataCellStyle="Normal"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table2214" displayName="Table2214" ref="B5:F44" headerRowCount="0" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
+  <tableColumns count="5">
+    <tableColumn id="1" name="Column1" headerRowDxfId="20" dataCellStyle="Normal"/>
+    <tableColumn id="2" name="Column2" headerRowDxfId="19" dataCellStyle="Normal"/>
+    <tableColumn id="3" name="Column3" headerRowDxfId="18" dataCellStyle="Normal"/>
+    <tableColumn id="4" name="Column4" headerRowDxfId="17" dataCellStyle="Normal"/>
+    <tableColumn id="5" name="Column5" headerRowDxfId="16" dataCellStyle="Normal"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Table3715" displayName="Table3715" ref="B46:F59" headerRowCount="0" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
+  <tableColumns count="5">
+    <tableColumn id="1" name="Column1" headerRowDxfId="15" dataCellStyle="Normal"/>
+    <tableColumn id="2" name="Column2" headerRowDxfId="14" dataCellStyle="Normal"/>
+    <tableColumn id="3" name="Column3" headerRowDxfId="13" dataCellStyle="Normal"/>
+    <tableColumn id="4" name="Column4" headerRowDxfId="12" dataCellStyle="Normal"/>
+    <tableColumn id="5" name="Column5" headerRowDxfId="11" dataCellStyle="Normal"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Table4816" displayName="Table4816" ref="H43:J55" headerRowCount="0" totalsRowShown="0">
+  <tableColumns count="3">
+    <tableColumn id="1" name="Column1"/>
+    <tableColumn id="2" name="Column2"/>
+    <tableColumn id="3" name="Column3"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Table5917" displayName="Table5917" ref="H5:J41" headerRowCount="0" totalsRowShown="0" tableBorderDxfId="10">
+  <tableColumns count="3">
+    <tableColumn id="1" name="Column1"/>
+    <tableColumn id="2" name="Column2"/>
+    <tableColumn id="3" name="Column3"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Table221218" displayName="Table221218" ref="L5:P99" headerRowCount="0" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
+  <tableColumns count="5">
+    <tableColumn id="1" name="Column1" headerRowDxfId="9" dataCellStyle="Normal"/>
+    <tableColumn id="2" name="Column2" headerRowDxfId="8" dataCellStyle="Normal"/>
+    <tableColumn id="3" name="Column3" headerRowDxfId="7" dataCellStyle="Normal"/>
+    <tableColumn id="4" name="Column4" headerRowDxfId="6" dataCellStyle="Normal"/>
+    <tableColumn id="5" name="Column5" headerRowDxfId="5" dataCellStyle="Normal"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Table371319" displayName="Table371319" ref="L101:P115" headerRowCount="0" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
+  <tableColumns count="5">
+    <tableColumn id="1" name="Column1" headerRowDxfId="4" dataCellStyle="Normal"/>
+    <tableColumn id="2" name="Column2" headerRowDxfId="3" dataCellStyle="Normal"/>
+    <tableColumn id="3" name="Column3" headerRowDxfId="2" dataCellStyle="Normal"/>
+    <tableColumn id="4" name="Column4" headerRowDxfId="1" dataCellStyle="Normal"/>
+    <tableColumn id="5" name="Column5" headerRowDxfId="0" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2272,11 +2776,11 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B102:F116" headerRowCount="0" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
   <tableColumns count="5">
-    <tableColumn id="1" name="Column1" headerRowDxfId="26" dataCellStyle="Normal"/>
-    <tableColumn id="2" name="Column2" headerRowDxfId="25" dataCellStyle="Normal"/>
-    <tableColumn id="3" name="Column3" headerRowDxfId="24" dataCellStyle="Normal"/>
-    <tableColumn id="4" name="Column4" headerRowDxfId="23" dataCellStyle="Normal"/>
-    <tableColumn id="5" name="Column5" headerRowDxfId="22" dataCellStyle="Normal"/>
+    <tableColumn id="1" name="Column1" headerRowDxfId="47" dataCellStyle="Normal"/>
+    <tableColumn id="2" name="Column2" headerRowDxfId="46" dataCellStyle="Normal"/>
+    <tableColumn id="3" name="Column3" headerRowDxfId="45" dataCellStyle="Normal"/>
+    <tableColumn id="4" name="Column4" headerRowDxfId="44" dataCellStyle="Normal"/>
+    <tableColumn id="5" name="Column5" headerRowDxfId="43" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2294,7 +2798,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="H5:J82" headerRowCount="0" totalsRowShown="0" tableBorderDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="H5:J82" headerRowCount="0" totalsRowShown="0" tableBorderDxfId="42">
   <tableColumns count="3">
     <tableColumn id="1" name="Column1"/>
     <tableColumn id="2" name="Column2"/>
@@ -2307,11 +2811,11 @@
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table22" displayName="Table22" ref="B5:F44" headerRowCount="0" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
   <tableColumns count="5">
-    <tableColumn id="1" name="Column1" headerRowDxfId="9" dataCellStyle="Normal"/>
-    <tableColumn id="2" name="Column2" headerRowDxfId="8" dataCellStyle="Normal"/>
-    <tableColumn id="3" name="Column3" headerRowDxfId="7" dataCellStyle="Normal"/>
-    <tableColumn id="4" name="Column4" headerRowDxfId="6" dataCellStyle="Normal"/>
-    <tableColumn id="5" name="Column5" headerRowDxfId="5" dataCellStyle="Normal"/>
+    <tableColumn id="1" name="Column1" headerRowDxfId="30" dataCellStyle="Normal"/>
+    <tableColumn id="2" name="Column2" headerRowDxfId="29" dataCellStyle="Normal"/>
+    <tableColumn id="3" name="Column3" headerRowDxfId="28" dataCellStyle="Normal"/>
+    <tableColumn id="4" name="Column4" headerRowDxfId="27" dataCellStyle="Normal"/>
+    <tableColumn id="5" name="Column5" headerRowDxfId="26" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2320,11 +2824,11 @@
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table37" displayName="Table37" ref="B46:F59" headerRowCount="0" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
   <tableColumns count="5">
-    <tableColumn id="1" name="Column1" headerRowDxfId="4" dataCellStyle="Normal"/>
-    <tableColumn id="2" name="Column2" headerRowDxfId="3" dataCellStyle="Normal"/>
-    <tableColumn id="3" name="Column3" headerRowDxfId="2" dataCellStyle="Normal"/>
-    <tableColumn id="4" name="Column4" headerRowDxfId="1" dataCellStyle="Normal"/>
-    <tableColumn id="5" name="Column5" headerRowDxfId="0" dataCellStyle="Normal"/>
+    <tableColumn id="1" name="Column1" headerRowDxfId="25" dataCellStyle="Normal"/>
+    <tableColumn id="2" name="Column2" headerRowDxfId="24" dataCellStyle="Normal"/>
+    <tableColumn id="3" name="Column3" headerRowDxfId="23" dataCellStyle="Normal"/>
+    <tableColumn id="4" name="Column4" headerRowDxfId="22" dataCellStyle="Normal"/>
+    <tableColumn id="5" name="Column5" headerRowDxfId="21" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2342,7 +2846,7 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table59" displayName="Table59" ref="H5:J41" headerRowCount="0" totalsRowShown="0" tableBorderDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table59" displayName="Table59" ref="H5:J41" headerRowCount="0" totalsRowShown="0" tableBorderDxfId="41">
   <tableColumns count="3">
     <tableColumn id="1" name="Column1"/>
     <tableColumn id="2" name="Column2"/>
@@ -2355,11 +2859,11 @@
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table2212" displayName="Table2212" ref="L5:P99" headerRowCount="0" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
   <tableColumns count="5">
-    <tableColumn id="1" name="Column1" headerRowDxfId="19" dataCellStyle="Normal"/>
-    <tableColumn id="2" name="Column2" headerRowDxfId="18" dataCellStyle="Normal"/>
-    <tableColumn id="3" name="Column3" headerRowDxfId="17" dataCellStyle="Normal"/>
-    <tableColumn id="4" name="Column4" headerRowDxfId="16" dataCellStyle="Normal"/>
-    <tableColumn id="5" name="Column5" headerRowDxfId="15" dataCellStyle="Normal"/>
+    <tableColumn id="1" name="Column1" headerRowDxfId="40" dataCellStyle="Normal"/>
+    <tableColumn id="2" name="Column2" headerRowDxfId="39" dataCellStyle="Normal"/>
+    <tableColumn id="3" name="Column3" headerRowDxfId="38" dataCellStyle="Normal"/>
+    <tableColumn id="4" name="Column4" headerRowDxfId="37" dataCellStyle="Normal"/>
+    <tableColumn id="5" name="Column5" headerRowDxfId="36" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5680,8 +6184,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7307,16 +7811,16 @@
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B42" s="23" t="s">
         <v>441</v>
       </c>
       <c r="C42" s="23" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D42" s="23" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E42" s="23">
         <v>13</v>
@@ -7348,16 +7852,16 @@
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B43" s="23" t="s">
         <v>441</v>
       </c>
       <c r="C43" s="23" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D43" s="23" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E43" s="23">
         <v>13</v>
@@ -7397,7 +7901,7 @@
         <v>445</v>
       </c>
       <c r="D44" s="23" t="s">
-        <v>446</v>
+        <v>450</v>
       </c>
       <c r="E44" s="23">
         <v>13</v>
@@ -8087,7 +8591,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="65" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="65" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="L65" t="s">
         <v>277</v>
       </c>
@@ -8104,7 +8608,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="66" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="66" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="L66" t="s">
         <v>277</v>
       </c>
@@ -8121,7 +8625,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="67" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="67" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="L67" t="s">
         <v>277</v>
       </c>
@@ -8138,7 +8642,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="68" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="68" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="L68" t="s">
         <v>277</v>
       </c>
@@ -8155,7 +8659,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="69" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="69" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="L69" t="s">
         <v>277</v>
       </c>
@@ -8173,7 +8677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="70" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="L70" t="s">
         <v>277</v>
       </c>
@@ -8190,7 +8694,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="71" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="71" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="L71" t="s">
         <v>277</v>
       </c>
@@ -8207,7 +8711,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="72" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="72" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="L72" t="s">
         <v>277</v>
       </c>
@@ -8224,7 +8728,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="73" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="73" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="L73" t="s">
         <v>277</v>
       </c>
@@ -8242,7 +8746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="74" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="L74" t="s">
         <v>277</v>
       </c>
@@ -8259,7 +8763,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="75" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="75" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="L75" t="s">
         <v>277</v>
       </c>
@@ -8276,7 +8780,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="76" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="76" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="L76" t="s">
         <v>277</v>
       </c>
@@ -8293,7 +8797,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="77" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="77" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="L77" t="s">
         <v>277</v>
       </c>
@@ -8311,7 +8815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="78" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="L78" t="s">
         <v>277</v>
       </c>
@@ -8329,7 +8833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="79" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="L79" t="s">
         <v>277</v>
       </c>
@@ -8346,7 +8850,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="80" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="80" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="L80" t="s">
         <v>277</v>
       </c>
@@ -8363,7 +8867,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="81" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="81" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="L81" t="s">
         <v>277</v>
       </c>
@@ -8380,7 +8884,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="82" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="82" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="L82" t="s">
         <v>277</v>
       </c>
@@ -8397,7 +8901,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="83" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="83" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="L83" t="s">
         <v>277</v>
       </c>
@@ -8414,7 +8918,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="84" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="84" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="L84" t="s">
         <v>277</v>
       </c>
@@ -8431,7 +8935,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="85" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="85" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="L85" t="s">
         <v>277</v>
       </c>
@@ -8448,7 +8952,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="86" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="86" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="L86" t="s">
         <v>277</v>
       </c>
@@ -8465,7 +8969,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="87" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="87" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="L87" t="s">
         <v>277</v>
       </c>
@@ -8482,7 +8986,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="88" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="88" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="L88" t="s">
         <v>277</v>
       </c>
@@ -8500,7 +9004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="89" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="L89" t="s">
         <v>277</v>
       </c>
@@ -8518,7 +9022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="90" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="L90" t="s">
         <v>277</v>
       </c>
@@ -8535,7 +9039,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="91" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="91" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="L91" t="s">
         <v>277</v>
       </c>
@@ -8553,7 +9057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="92" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="L92" t="s">
         <v>277</v>
       </c>
@@ -8571,7 +9075,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="93" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="93" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="L93" t="s">
         <v>277</v>
       </c>
@@ -8589,7 +9093,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="94" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="94" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="L94" t="s">
         <v>277</v>
       </c>
@@ -8606,7 +9110,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="95" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="95" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="L95" t="s">
         <v>277</v>
       </c>
@@ -8624,7 +9128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="96" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="L96" t="s">
         <v>277</v>
       </c>
@@ -8642,7 +9146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="97" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="L97" t="s">
         <v>277</v>
       </c>
@@ -8660,7 +9164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="98" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="L98" t="s">
         <v>277</v>
       </c>
@@ -8678,7 +9182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="99" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="L99" t="s">
         <v>277</v>
       </c>
@@ -8696,7 +9200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="100" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="L100" s="9" t="s">
         <v>427</v>
       </c>
@@ -8705,7 +9209,7 @@
       <c r="O100" s="13"/>
       <c r="P100" s="10"/>
     </row>
-    <row r="101" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="101" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="L101" t="s">
         <v>321</v>
       </c>
@@ -8723,7 +9227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="102" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="L102" t="s">
         <v>321</v>
       </c>
@@ -8741,7 +9245,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="103" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="103" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="L103" t="s">
         <v>321</v>
       </c>
@@ -8759,7 +9263,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="104" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="104" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="L104" t="s">
         <v>321</v>
       </c>
@@ -8777,7 +9281,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="105" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="105" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="L105" t="s">
         <v>321</v>
       </c>
@@ -8795,7 +9299,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="106" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="106" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="L106" t="s">
         <v>321</v>
       </c>
@@ -8813,7 +9317,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="107" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="107" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="L107" t="s">
         <v>321</v>
       </c>
@@ -8831,7 +9335,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="108" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="108" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="L108" t="s">
         <v>321</v>
       </c>
@@ -8849,7 +9353,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="109" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="109" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="L109" t="s">
         <v>321</v>
       </c>
@@ -8867,7 +9371,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="110" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="110" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="L110" t="s">
         <v>321</v>
       </c>
@@ -8884,7 +9388,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="111" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="111" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="L111" t="s">
         <v>321</v>
       </c>
@@ -8902,7 +9406,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="112" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="112" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="L112" t="s">
         <v>277</v>
       </c>
@@ -8919,7 +9423,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="113" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="113" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="L113" t="s">
         <v>321</v>
       </c>
@@ -8937,7 +9441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="114" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="L114" t="s">
         <v>321</v>
       </c>
@@ -8955,7 +9459,3323 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="115" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="115" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L115" t="s">
+        <v>321</v>
+      </c>
+      <c r="M115" t="s">
+        <v>326</v>
+      </c>
+      <c r="N115" t="s">
+        <v>326</v>
+      </c>
+      <c r="O115">
+        <v>3</v>
+      </c>
+      <c r="P115">
+        <f>R43</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="L2:P2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="6">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P115"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.7109375" customWidth="1"/>
+    <col min="5" max="5" width="11" style="14" customWidth="1"/>
+    <col min="6" max="6" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" customWidth="1"/>
+    <col min="8" max="8" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11" customWidth="1"/>
+    <col min="13" max="13" width="15" customWidth="1"/>
+    <col min="14" max="14" width="31.7109375" customWidth="1"/>
+    <col min="15" max="15" width="11" style="14" customWidth="1"/>
+    <col min="16" max="16" width="24.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="6"/>
+      <c r="H1" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="L1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="6"/>
+    </row>
+    <row r="2" spans="1:16" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
+        <v>430</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>431</v>
+      </c>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="H2" s="18" t="s">
+        <v>433</v>
+      </c>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="L2" s="21" t="s">
+        <v>431</v>
+      </c>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="22"/>
+      <c r="P2" s="22"/>
+    </row>
+    <row r="3" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="20"/>
+      <c r="B3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>426</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="O3" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4"/>
+      <c r="B4" s="9" t="s">
+        <v>428</v>
+      </c>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="10"/>
+      <c r="G4"/>
+      <c r="H4" s="9" t="s">
+        <v>428</v>
+      </c>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="L4" s="9" t="s">
+        <v>428</v>
+      </c>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="13"/>
+      <c r="P4" s="10"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>277</v>
+      </c>
+      <c r="C5" t="s">
+        <v>432</v>
+      </c>
+      <c r="E5">
+        <v>10</v>
+      </c>
+      <c r="F5" t="str">
+        <f>Table5917[[#This Row],[Column1]]</f>
+        <v>MessageFormat</v>
+      </c>
+      <c r="H5" t="s">
+        <v>432</v>
+      </c>
+      <c r="I5"/>
+      <c r="J5" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="L5" t="s">
+        <v>222</v>
+      </c>
+      <c r="M5" t="s">
+        <v>220</v>
+      </c>
+      <c r="N5" t="s">
+        <v>336</v>
+      </c>
+      <c r="O5">
+        <v>3</v>
+      </c>
+      <c r="P5" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>277</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" t="str">
+        <f>Table5917[[#This Row],[Column1]]</f>
+        <v>MessageType</v>
+      </c>
+      <c r="H6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6"/>
+      <c r="J6" s="17" t="s">
+        <v>217</v>
+      </c>
+      <c r="L6" t="s">
+        <v>222</v>
+      </c>
+      <c r="M6" t="s">
+        <v>221</v>
+      </c>
+      <c r="N6" t="s">
+        <v>337</v>
+      </c>
+      <c r="O6">
+        <v>35</v>
+      </c>
+      <c r="P6" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>277</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>113</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7" t="str">
+        <f>Table5917[[#This Row],[Column1]]</f>
+        <v>IsTestMessage</v>
+      </c>
+      <c r="H7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7" t="s">
+        <v>113</v>
+      </c>
+      <c r="J7" t="s">
+        <v>435</v>
+      </c>
+      <c r="L7" t="s">
+        <v>222</v>
+      </c>
+      <c r="M7" t="s">
+        <v>223</v>
+      </c>
+      <c r="N7" t="s">
+        <v>338</v>
+      </c>
+      <c r="O7">
+        <v>35</v>
+      </c>
+      <c r="P7" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>277</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>112</v>
+      </c>
+      <c r="E8">
+        <v>12</v>
+      </c>
+      <c r="F8" t="str">
+        <f>Table5917[[#This Row],[Column1]]</f>
+        <v>MessageReference</v>
+      </c>
+      <c r="H8" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8" t="s">
+        <v>112</v>
+      </c>
+      <c r="L8" t="s">
+        <v>222</v>
+      </c>
+      <c r="M8" t="s">
+        <v>224</v>
+      </c>
+      <c r="N8" t="s">
+        <v>339</v>
+      </c>
+      <c r="O8">
+        <v>9</v>
+      </c>
+      <c r="P8" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>277</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
+        <v>124</v>
+      </c>
+      <c r="E9">
+        <v>6</v>
+      </c>
+      <c r="F9" t="str">
+        <f>Table5917[[#This Row],[Column1]]</f>
+        <v>OrderNumberBuyer</v>
+      </c>
+      <c r="H9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I9" t="s">
+        <v>124</v>
+      </c>
+      <c r="J9"/>
+      <c r="L9" t="s">
+        <v>222</v>
+      </c>
+      <c r="M9" t="s">
+        <v>225</v>
+      </c>
+      <c r="N9" t="s">
+        <v>340</v>
+      </c>
+      <c r="O9">
+        <v>8</v>
+      </c>
+      <c r="P9" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>277</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" t="s">
+        <v>125</v>
+      </c>
+      <c r="E10">
+        <v>16</v>
+      </c>
+      <c r="F10" t="str">
+        <f>Table5917[[#This Row],[Column1]]</f>
+        <v>OrderDate</v>
+      </c>
+      <c r="H10" t="s">
+        <v>19</v>
+      </c>
+      <c r="I10" t="s">
+        <v>125</v>
+      </c>
+      <c r="J10" t="s">
+        <v>434</v>
+      </c>
+      <c r="L10" t="s">
+        <v>222</v>
+      </c>
+      <c r="M10" t="s">
+        <v>226</v>
+      </c>
+      <c r="N10" t="s">
+        <v>341</v>
+      </c>
+      <c r="O10">
+        <v>3</v>
+      </c>
+      <c r="P10" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>277</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>114</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11" t="str">
+        <f>Table5917[[#This Row],[Column1]]</f>
+        <v>IsCrossdock</v>
+      </c>
+      <c r="H11" t="s">
+        <v>8</v>
+      </c>
+      <c r="I11" t="s">
+        <v>114</v>
+      </c>
+      <c r="J11" t="s">
+        <v>435</v>
+      </c>
+      <c r="L11" t="s">
+        <v>222</v>
+      </c>
+      <c r="M11" t="s">
+        <v>227</v>
+      </c>
+      <c r="N11" t="s">
+        <v>342</v>
+      </c>
+      <c r="O11">
+        <v>6</v>
+      </c>
+      <c r="P11" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>277</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
+        <v>118</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12" t="str">
+        <f>Table5917[[#This Row],[Column1]]</f>
+        <v>IsCallOffOrder</v>
+      </c>
+      <c r="H12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I12" t="s">
+        <v>118</v>
+      </c>
+      <c r="J12" t="s">
+        <v>435</v>
+      </c>
+      <c r="L12" t="s">
+        <v>222</v>
+      </c>
+      <c r="M12" t="s">
+        <v>228</v>
+      </c>
+      <c r="N12" t="s">
+        <v>343</v>
+      </c>
+      <c r="O12">
+        <v>19</v>
+      </c>
+      <c r="P12" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>277</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
+        <v>128</v>
+      </c>
+      <c r="E13">
+        <v>12</v>
+      </c>
+      <c r="F13" t="str">
+        <f>Table5917[[#This Row],[Column1]]</f>
+        <v>RequestedDeliveryDate</v>
+      </c>
+      <c r="H13" t="s">
+        <v>22</v>
+      </c>
+      <c r="I13" t="s">
+        <v>128</v>
+      </c>
+      <c r="J13" t="s">
+        <v>434</v>
+      </c>
+      <c r="L13" t="s">
+        <v>222</v>
+      </c>
+      <c r="M13" t="s">
+        <v>229</v>
+      </c>
+      <c r="N13" t="s">
+        <v>344</v>
+      </c>
+      <c r="O13">
+        <v>3</v>
+      </c>
+      <c r="P13" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>277</v>
+      </c>
+      <c r="C14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" t="s">
+        <v>126</v>
+      </c>
+      <c r="E14">
+        <v>12</v>
+      </c>
+      <c r="F14" t="str">
+        <f>Table5917[[#This Row],[Column1]]</f>
+        <v>EarliestDeliveryDate</v>
+      </c>
+      <c r="H14" t="s">
+        <v>20</v>
+      </c>
+      <c r="I14" t="s">
+        <v>126</v>
+      </c>
+      <c r="J14" t="s">
+        <v>434</v>
+      </c>
+      <c r="L14" t="s">
+        <v>222</v>
+      </c>
+      <c r="M14" t="s">
+        <v>230</v>
+      </c>
+      <c r="N14" t="s">
+        <v>345</v>
+      </c>
+      <c r="O14">
+        <v>14</v>
+      </c>
+      <c r="P14" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>277</v>
+      </c>
+      <c r="C15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" t="s">
+        <v>127</v>
+      </c>
+      <c r="E15">
+        <v>12</v>
+      </c>
+      <c r="F15" t="str">
+        <f>Table5917[[#This Row],[Column1]]</f>
+        <v>LatestDeliveryDate</v>
+      </c>
+      <c r="H15" t="s">
+        <v>21</v>
+      </c>
+      <c r="I15" t="s">
+        <v>127</v>
+      </c>
+      <c r="J15" t="s">
+        <v>434</v>
+      </c>
+      <c r="L15" t="s">
+        <v>222</v>
+      </c>
+      <c r="M15" t="s">
+        <v>231</v>
+      </c>
+      <c r="N15" t="s">
+        <v>346</v>
+      </c>
+      <c r="O15">
+        <v>17</v>
+      </c>
+      <c r="P15" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>277</v>
+      </c>
+      <c r="C16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" t="s">
+        <v>116</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16" t="str">
+        <f>Table5917[[#This Row],[Column1]]</f>
+        <v>IsShopInstallation</v>
+      </c>
+      <c r="H16" t="s">
+        <v>10</v>
+      </c>
+      <c r="I16" t="s">
+        <v>116</v>
+      </c>
+      <c r="J16" t="s">
+        <v>435</v>
+      </c>
+      <c r="L16" t="s">
+        <v>222</v>
+      </c>
+      <c r="M16" t="s">
+        <v>232</v>
+      </c>
+      <c r="N16" t="s">
+        <v>347</v>
+      </c>
+      <c r="O16">
+        <v>3</v>
+      </c>
+      <c r="P16" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>277</v>
+      </c>
+      <c r="C17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" t="s">
+        <v>122</v>
+      </c>
+      <c r="E17">
+        <v>6</v>
+      </c>
+      <c r="F17" t="str">
+        <f>Table5917[[#This Row],[Column1]]</f>
+        <v>BlanketOrderNumber</v>
+      </c>
+      <c r="H17" t="s">
+        <v>16</v>
+      </c>
+      <c r="I17" t="s">
+        <v>122</v>
+      </c>
+      <c r="J17"/>
+      <c r="L17" t="s">
+        <v>222</v>
+      </c>
+      <c r="M17" t="s">
+        <v>233</v>
+      </c>
+      <c r="N17" t="s">
+        <v>348</v>
+      </c>
+      <c r="O17">
+        <v>6</v>
+      </c>
+      <c r="P17" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>277</v>
+      </c>
+      <c r="C18" t="s">
+        <v>70</v>
+      </c>
+      <c r="D18" t="s">
+        <v>176</v>
+      </c>
+      <c r="E18">
+        <v>35</v>
+      </c>
+      <c r="F18" t="str">
+        <f>Table5917[[#This Row],[Column1]]</f>
+        <v>ConsumerReference</v>
+      </c>
+      <c r="H18" t="s">
+        <v>70</v>
+      </c>
+      <c r="I18" t="s">
+        <v>176</v>
+      </c>
+      <c r="L18" t="s">
+        <v>222</v>
+      </c>
+      <c r="M18" t="s">
+        <v>234</v>
+      </c>
+      <c r="N18" t="s">
+        <v>349</v>
+      </c>
+      <c r="O18">
+        <v>35</v>
+      </c>
+      <c r="P18" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>277</v>
+      </c>
+      <c r="C19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" t="s">
+        <v>123</v>
+      </c>
+      <c r="E19">
+        <v>35</v>
+      </c>
+      <c r="F19" t="str">
+        <f>Table5917[[#This Row],[Column1]]</f>
+        <v>ActionNumber</v>
+      </c>
+      <c r="H19" t="s">
+        <v>17</v>
+      </c>
+      <c r="I19" t="s">
+        <v>123</v>
+      </c>
+      <c r="J19"/>
+      <c r="L19" t="s">
+        <v>222</v>
+      </c>
+      <c r="M19" t="s">
+        <v>235</v>
+      </c>
+      <c r="N19" t="s">
+        <v>350</v>
+      </c>
+      <c r="O19">
+        <v>1</v>
+      </c>
+      <c r="P19" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>277</v>
+      </c>
+      <c r="C20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" t="s">
+        <v>130</v>
+      </c>
+      <c r="E20">
+        <v>35</v>
+      </c>
+      <c r="F20" t="str">
+        <f>Table5917[[#This Row],[Column1]]</f>
+        <v>BuyerGLN</v>
+      </c>
+      <c r="H20" t="s">
+        <v>24</v>
+      </c>
+      <c r="I20" t="s">
+        <v>130</v>
+      </c>
+      <c r="J20"/>
+      <c r="L20" t="s">
+        <v>236</v>
+      </c>
+      <c r="M20" t="s">
+        <v>237</v>
+      </c>
+      <c r="N20" t="s">
+        <v>351</v>
+      </c>
+      <c r="O20">
+        <v>35</v>
+      </c>
+      <c r="P20" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>277</v>
+      </c>
+      <c r="C21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" t="s">
+        <v>132</v>
+      </c>
+      <c r="E21">
+        <v>9</v>
+      </c>
+      <c r="F21" t="str">
+        <f>Table5917[[#This Row],[Column1]]</f>
+        <v>BuyerID</v>
+      </c>
+      <c r="H21" t="s">
+        <v>26</v>
+      </c>
+      <c r="I21" t="s">
+        <v>132</v>
+      </c>
+      <c r="L21" t="s">
+        <v>236</v>
+      </c>
+      <c r="M21" t="s">
+        <v>238</v>
+      </c>
+      <c r="N21" t="s">
+        <v>352</v>
+      </c>
+      <c r="O21">
+        <v>9</v>
+      </c>
+      <c r="P21" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>277</v>
+      </c>
+      <c r="C22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" t="s">
+        <v>129</v>
+      </c>
+      <c r="E22">
+        <v>35</v>
+      </c>
+      <c r="F22" t="str">
+        <f>Table5917[[#This Row],[Column1]]</f>
+        <v>Buyer</v>
+      </c>
+      <c r="H22" t="s">
+        <v>25</v>
+      </c>
+      <c r="I22" t="s">
+        <v>131</v>
+      </c>
+      <c r="J22"/>
+      <c r="L22" t="s">
+        <v>236</v>
+      </c>
+      <c r="M22" t="s">
+        <v>239</v>
+      </c>
+      <c r="N22" t="s">
+        <v>353</v>
+      </c>
+      <c r="O22">
+        <v>35</v>
+      </c>
+      <c r="P22" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>277</v>
+      </c>
+      <c r="C23" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" t="s">
+        <v>134</v>
+      </c>
+      <c r="E23">
+        <v>13</v>
+      </c>
+      <c r="F23" t="str">
+        <f>Table5917[[#This Row],[Column1]]</f>
+        <v>SupplierGLN</v>
+      </c>
+      <c r="H23" t="s">
+        <v>28</v>
+      </c>
+      <c r="I23" t="s">
+        <v>134</v>
+      </c>
+      <c r="J23"/>
+      <c r="L23" t="s">
+        <v>236</v>
+      </c>
+      <c r="M23" t="s">
+        <v>240</v>
+      </c>
+      <c r="N23" t="s">
+        <v>354</v>
+      </c>
+      <c r="O23">
+        <v>35</v>
+      </c>
+      <c r="P23">
+        <f>R9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>277</v>
+      </c>
+      <c r="C24" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24" t="s">
+        <v>133</v>
+      </c>
+      <c r="E24">
+        <v>35</v>
+      </c>
+      <c r="F24" t="str">
+        <f>Table5917[[#This Row],[Column1]]</f>
+        <v>Supplier</v>
+      </c>
+      <c r="H24" t="s">
+        <v>27</v>
+      </c>
+      <c r="I24" t="s">
+        <v>133</v>
+      </c>
+      <c r="L24" t="s">
+        <v>236</v>
+      </c>
+      <c r="M24" t="s">
+        <v>241</v>
+      </c>
+      <c r="N24" t="s">
+        <v>355</v>
+      </c>
+      <c r="O24">
+        <v>20</v>
+      </c>
+      <c r="P24" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>277</v>
+      </c>
+      <c r="C25" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" t="s">
+        <v>136</v>
+      </c>
+      <c r="E25">
+        <v>35</v>
+      </c>
+      <c r="F25" t="str">
+        <f>Table5917[[#This Row],[Column1]]</f>
+        <v>Invoicee</v>
+      </c>
+      <c r="H25" t="s">
+        <v>30</v>
+      </c>
+      <c r="I25" t="s">
+        <v>136</v>
+      </c>
+      <c r="J25"/>
+      <c r="L25" t="s">
+        <v>236</v>
+      </c>
+      <c r="M25" t="s">
+        <v>242</v>
+      </c>
+      <c r="N25" t="s">
+        <v>356</v>
+      </c>
+      <c r="O25">
+        <v>10</v>
+      </c>
+      <c r="P25" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>277</v>
+      </c>
+      <c r="C26" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" t="s">
+        <v>137</v>
+      </c>
+      <c r="E26">
+        <v>13</v>
+      </c>
+      <c r="F26" t="str">
+        <f>Table5917[[#This Row],[Column1]]</f>
+        <v>InvoiceeGLN</v>
+      </c>
+      <c r="H26" t="s">
+        <v>31</v>
+      </c>
+      <c r="I26" t="s">
+        <v>137</v>
+      </c>
+      <c r="J26"/>
+      <c r="L26" t="s">
+        <v>236</v>
+      </c>
+      <c r="M26" t="s">
+        <v>243</v>
+      </c>
+      <c r="N26" t="s">
+        <v>357</v>
+      </c>
+      <c r="O26">
+        <v>10</v>
+      </c>
+      <c r="P26" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>277</v>
+      </c>
+      <c r="C27" t="s">
+        <v>40</v>
+      </c>
+      <c r="D27" t="s">
+        <v>146</v>
+      </c>
+      <c r="E27">
+        <v>35</v>
+      </c>
+      <c r="F27" t="str">
+        <f>Table5917[[#This Row],[Column1]]</f>
+        <v>DeliveryParty</v>
+      </c>
+      <c r="H27" t="s">
+        <v>40</v>
+      </c>
+      <c r="I27" t="s">
+        <v>146</v>
+      </c>
+      <c r="J27"/>
+      <c r="L27" t="s">
+        <v>244</v>
+      </c>
+      <c r="M27" t="s">
+        <v>28</v>
+      </c>
+      <c r="N27" t="s">
+        <v>28</v>
+      </c>
+      <c r="O27">
+        <v>13</v>
+      </c>
+      <c r="P27">
+        <f>R23</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>277</v>
+      </c>
+      <c r="C28" t="s">
+        <v>42</v>
+      </c>
+      <c r="D28" t="s">
+        <v>148</v>
+      </c>
+      <c r="E28">
+        <v>13</v>
+      </c>
+      <c r="F28" t="str">
+        <f>Table5917[[#This Row],[Column1]]</f>
+        <v>DeliveryPartyGLN</v>
+      </c>
+      <c r="H28" t="s">
+        <v>42</v>
+      </c>
+      <c r="I28" t="s">
+        <v>148</v>
+      </c>
+      <c r="J28"/>
+      <c r="L28" t="s">
+        <v>245</v>
+      </c>
+      <c r="M28" t="s">
+        <v>246</v>
+      </c>
+      <c r="N28" t="s">
+        <v>358</v>
+      </c>
+      <c r="O28">
+        <v>13</v>
+      </c>
+      <c r="P28" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>277</v>
+      </c>
+      <c r="C29" t="s">
+        <v>43</v>
+      </c>
+      <c r="D29" t="s">
+        <v>149</v>
+      </c>
+      <c r="E29">
+        <v>35</v>
+      </c>
+      <c r="F29" t="str">
+        <f>Table5917[[#This Row],[Column1]]</f>
+        <v>DeliveryPartyAddress</v>
+      </c>
+      <c r="H29" t="s">
+        <v>43</v>
+      </c>
+      <c r="I29" t="s">
+        <v>149</v>
+      </c>
+      <c r="J29"/>
+      <c r="L29" t="s">
+        <v>247</v>
+      </c>
+      <c r="M29" t="s">
+        <v>248</v>
+      </c>
+      <c r="N29" t="s">
+        <v>359</v>
+      </c>
+      <c r="O29">
+        <v>8</v>
+      </c>
+      <c r="P29" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>277</v>
+      </c>
+      <c r="C30" t="s">
+        <v>45</v>
+      </c>
+      <c r="D30" t="s">
+        <v>151</v>
+      </c>
+      <c r="E30">
+        <v>7</v>
+      </c>
+      <c r="F30" t="str">
+        <f>Table5917[[#This Row],[Column1]]</f>
+        <v>DeliveryPartyZipcode</v>
+      </c>
+      <c r="H30" t="s">
+        <v>45</v>
+      </c>
+      <c r="I30" t="s">
+        <v>151</v>
+      </c>
+      <c r="J30"/>
+      <c r="L30" t="s">
+        <v>247</v>
+      </c>
+      <c r="M30" t="s">
+        <v>249</v>
+      </c>
+      <c r="N30" t="s">
+        <v>360</v>
+      </c>
+      <c r="O30">
+        <v>13</v>
+      </c>
+      <c r="P30" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>277</v>
+      </c>
+      <c r="C31" t="s">
+        <v>44</v>
+      </c>
+      <c r="D31" t="s">
+        <v>150</v>
+      </c>
+      <c r="E31">
+        <v>35</v>
+      </c>
+      <c r="F31" t="str">
+        <f>Table5917[[#This Row],[Column1]]</f>
+        <v>DeliveryPartyCity</v>
+      </c>
+      <c r="H31" t="s">
+        <v>44</v>
+      </c>
+      <c r="I31" t="s">
+        <v>150</v>
+      </c>
+      <c r="J31"/>
+      <c r="L31" t="s">
+        <v>247</v>
+      </c>
+      <c r="M31" t="s">
+        <v>250</v>
+      </c>
+      <c r="N31" t="s">
+        <v>361</v>
+      </c>
+      <c r="O31">
+        <v>5</v>
+      </c>
+      <c r="P31" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>277</v>
+      </c>
+      <c r="C32" t="s">
+        <v>46</v>
+      </c>
+      <c r="D32" t="s">
+        <v>152</v>
+      </c>
+      <c r="E32">
+        <v>35</v>
+      </c>
+      <c r="F32" t="str">
+        <f>Table5917[[#This Row],[Column1]]</f>
+        <v>DeliveryPartyCountry</v>
+      </c>
+      <c r="H32" t="s">
+        <v>46</v>
+      </c>
+      <c r="I32" t="s">
+        <v>152</v>
+      </c>
+      <c r="J32"/>
+      <c r="L32" t="s">
+        <v>247</v>
+      </c>
+      <c r="M32" t="s">
+        <v>251</v>
+      </c>
+      <c r="N32" t="s">
+        <v>362</v>
+      </c>
+      <c r="O32">
+        <v>1</v>
+      </c>
+      <c r="P32" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>277</v>
+      </c>
+      <c r="C33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D33" t="s">
+        <v>141</v>
+      </c>
+      <c r="E33">
+        <v>13</v>
+      </c>
+      <c r="F33" t="str">
+        <f>Table5917[[#This Row],[Column1]]</f>
+        <v>ShipFromPartyGLN</v>
+      </c>
+      <c r="H33" t="s">
+        <v>35</v>
+      </c>
+      <c r="I33" t="s">
+        <v>141</v>
+      </c>
+      <c r="J33"/>
+      <c r="L33" t="s">
+        <v>247</v>
+      </c>
+      <c r="M33" t="s">
+        <v>252</v>
+      </c>
+      <c r="N33" t="s">
+        <v>363</v>
+      </c>
+      <c r="O33">
+        <v>35</v>
+      </c>
+      <c r="P33" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>277</v>
+      </c>
+      <c r="C34" t="s">
+        <v>47</v>
+      </c>
+      <c r="D34" t="s">
+        <v>153</v>
+      </c>
+      <c r="E34">
+        <v>35</v>
+      </c>
+      <c r="F34" t="str">
+        <f>Table5917[[#This Row],[Column1]]</f>
+        <v>UltimateConsignee</v>
+      </c>
+      <c r="H34" t="s">
+        <v>47</v>
+      </c>
+      <c r="I34" t="s">
+        <v>153</v>
+      </c>
+      <c r="J34"/>
+      <c r="L34" t="s">
+        <v>247</v>
+      </c>
+      <c r="M34" t="s">
+        <v>253</v>
+      </c>
+      <c r="N34" t="s">
+        <v>364</v>
+      </c>
+      <c r="O34">
+        <v>35</v>
+      </c>
+      <c r="P34" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>277</v>
+      </c>
+      <c r="C35" t="s">
+        <v>49</v>
+      </c>
+      <c r="D35" t="s">
+        <v>155</v>
+      </c>
+      <c r="E35">
+        <v>13</v>
+      </c>
+      <c r="F35" t="str">
+        <f>Table5917[[#This Row],[Column1]]</f>
+        <v>UltimateConsigneeGLN</v>
+      </c>
+      <c r="H35" t="s">
+        <v>49</v>
+      </c>
+      <c r="I35" t="s">
+        <v>155</v>
+      </c>
+      <c r="J35"/>
+      <c r="L35" t="s">
+        <v>254</v>
+      </c>
+      <c r="M35" t="s">
+        <v>255</v>
+      </c>
+      <c r="N35" t="s">
+        <v>365</v>
+      </c>
+      <c r="O35">
+        <v>13</v>
+      </c>
+      <c r="P35" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>277</v>
+      </c>
+      <c r="C36" t="s">
+        <v>50</v>
+      </c>
+      <c r="D36" t="s">
+        <v>156</v>
+      </c>
+      <c r="E36">
+        <v>35</v>
+      </c>
+      <c r="F36" t="str">
+        <f>Table5917[[#This Row],[Column1]]</f>
+        <v>UltimateConsigneeAddress</v>
+      </c>
+      <c r="H36" t="s">
+        <v>50</v>
+      </c>
+      <c r="I36" t="s">
+        <v>156</v>
+      </c>
+      <c r="J36"/>
+      <c r="L36" t="s">
+        <v>254</v>
+      </c>
+      <c r="M36" t="s">
+        <v>256</v>
+      </c>
+      <c r="N36" t="s">
+        <v>366</v>
+      </c>
+      <c r="O36">
+        <v>1</v>
+      </c>
+      <c r="P36" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>277</v>
+      </c>
+      <c r="C37" t="s">
+        <v>436</v>
+      </c>
+      <c r="D37" t="s">
+        <v>437</v>
+      </c>
+      <c r="E37">
+        <v>35</v>
+      </c>
+      <c r="F37" t="str">
+        <f>Table5917[[#This Row],[Column1]]</f>
+        <v>UltimateConsigneeZipcode</v>
+      </c>
+      <c r="H37" t="s">
+        <v>436</v>
+      </c>
+      <c r="I37" t="s">
+        <v>437</v>
+      </c>
+      <c r="J37"/>
+      <c r="L37" t="s">
+        <v>254</v>
+      </c>
+      <c r="M37" t="s">
+        <v>257</v>
+      </c>
+      <c r="N37" t="s">
+        <v>367</v>
+      </c>
+      <c r="O37">
+        <v>8</v>
+      </c>
+      <c r="P37" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>277</v>
+      </c>
+      <c r="C38" t="s">
+        <v>51</v>
+      </c>
+      <c r="D38" t="s">
+        <v>157</v>
+      </c>
+      <c r="E38">
+        <v>35</v>
+      </c>
+      <c r="F38" t="str">
+        <f>Table5917[[#This Row],[Column1]]</f>
+        <v>UltimateConsigneeCity</v>
+      </c>
+      <c r="H38" t="s">
+        <v>51</v>
+      </c>
+      <c r="I38" t="s">
+        <v>157</v>
+      </c>
+      <c r="J38"/>
+      <c r="L38" t="s">
+        <v>254</v>
+      </c>
+      <c r="M38" t="s">
+        <v>258</v>
+      </c>
+      <c r="N38" t="s">
+        <v>368</v>
+      </c>
+      <c r="O38">
+        <v>1</v>
+      </c>
+      <c r="P38" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>277</v>
+      </c>
+      <c r="C39" t="s">
+        <v>52</v>
+      </c>
+      <c r="D39" t="s">
+        <v>158</v>
+      </c>
+      <c r="E39">
+        <v>35</v>
+      </c>
+      <c r="F39" t="str">
+        <f>Table5917[[#This Row],[Column1]]</f>
+        <v>UltimateConsigneeCountry</v>
+      </c>
+      <c r="H39" t="s">
+        <v>52</v>
+      </c>
+      <c r="I39" t="s">
+        <v>158</v>
+      </c>
+      <c r="J39"/>
+      <c r="L39" t="s">
+        <v>254</v>
+      </c>
+      <c r="M39" t="s">
+        <v>259</v>
+      </c>
+      <c r="N39" t="s">
+        <v>369</v>
+      </c>
+      <c r="O39">
+        <v>3</v>
+      </c>
+      <c r="P39" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>277</v>
+      </c>
+      <c r="C40" t="s">
+        <v>9</v>
+      </c>
+      <c r="D40" t="s">
+        <v>115</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="F40" t="str">
+        <f>Table5917[[#This Row],[Column1]]</f>
+        <v>IsUrgent</v>
+      </c>
+      <c r="H40" t="s">
+        <v>9</v>
+      </c>
+      <c r="I40" t="s">
+        <v>115</v>
+      </c>
+      <c r="J40" t="s">
+        <v>435</v>
+      </c>
+      <c r="L40" t="s">
+        <v>254</v>
+      </c>
+      <c r="M40" t="s">
+        <v>260</v>
+      </c>
+      <c r="N40" t="s">
+        <v>370</v>
+      </c>
+      <c r="O40">
+        <v>13</v>
+      </c>
+      <c r="P40" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>277</v>
+      </c>
+      <c r="C41" t="s">
+        <v>13</v>
+      </c>
+      <c r="D41" t="s">
+        <v>119</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+      <c r="F41" t="str">
+        <f>Table5917[[#This Row],[Column1]]</f>
+        <v>IsBackhauling</v>
+      </c>
+      <c r="H41" t="s">
+        <v>13</v>
+      </c>
+      <c r="I41" t="s">
+        <v>119</v>
+      </c>
+      <c r="J41" t="s">
+        <v>435</v>
+      </c>
+      <c r="L41" t="s">
+        <v>254</v>
+      </c>
+      <c r="M41" t="s">
+        <v>261</v>
+      </c>
+      <c r="N41" t="s">
+        <v>371</v>
+      </c>
+      <c r="O41">
+        <v>3</v>
+      </c>
+      <c r="P41" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>448</v>
+      </c>
+      <c r="B42" s="23" t="s">
+        <v>441</v>
+      </c>
+      <c r="C42" s="23" t="s">
+        <v>447</v>
+      </c>
+      <c r="D42" s="23" t="s">
+        <v>446</v>
+      </c>
+      <c r="E42" s="23">
+        <v>13</v>
+      </c>
+      <c r="F42" s="24" t="str">
+        <f>H26</f>
+        <v>InvoiceeGLN</v>
+      </c>
+      <c r="H42" s="15" t="s">
+        <v>427</v>
+      </c>
+      <c r="I42" s="16"/>
+      <c r="J42" s="15"/>
+      <c r="L42" t="s">
+        <v>254</v>
+      </c>
+      <c r="M42" t="s">
+        <v>262</v>
+      </c>
+      <c r="N42" t="s">
+        <v>372</v>
+      </c>
+      <c r="O42">
+        <v>1</v>
+      </c>
+      <c r="P42" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>449</v>
+      </c>
+      <c r="B43" s="23" t="s">
+        <v>441</v>
+      </c>
+      <c r="C43" s="23" t="s">
+        <v>447</v>
+      </c>
+      <c r="D43" s="23" t="s">
+        <v>446</v>
+      </c>
+      <c r="E43" s="23">
+        <v>13</v>
+      </c>
+      <c r="F43" s="24" t="str">
+        <f>CONCATENATE(H28, " or ", H20)</f>
+        <v>DeliveryPartyGLN or BuyerGLN</v>
+      </c>
+      <c r="H43" t="s">
+        <v>82</v>
+      </c>
+      <c r="I43" t="s">
+        <v>188</v>
+      </c>
+      <c r="J43"/>
+      <c r="L43" t="s">
+        <v>254</v>
+      </c>
+      <c r="M43" t="s">
+        <v>263</v>
+      </c>
+      <c r="N43" t="s">
+        <v>373</v>
+      </c>
+      <c r="O43">
+        <v>8</v>
+      </c>
+      <c r="P43" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B44" s="23" t="s">
+        <v>442</v>
+      </c>
+      <c r="C44" s="23" t="s">
+        <v>445</v>
+      </c>
+      <c r="D44" s="23" t="s">
+        <v>450</v>
+      </c>
+      <c r="E44" s="23">
+        <v>13</v>
+      </c>
+      <c r="F44" s="24" t="str">
+        <f>H20</f>
+        <v>BuyerGLN</v>
+      </c>
+      <c r="H44" t="s">
+        <v>85</v>
+      </c>
+      <c r="I44" t="s">
+        <v>191</v>
+      </c>
+      <c r="J44"/>
+      <c r="L44" t="s">
+        <v>254</v>
+      </c>
+      <c r="M44" t="s">
+        <v>264</v>
+      </c>
+      <c r="N44" t="s">
+        <v>363</v>
+      </c>
+      <c r="O44">
+        <v>35</v>
+      </c>
+      <c r="P44" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B45" s="9" t="s">
+        <v>427</v>
+      </c>
+      <c r="C45" s="10"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="10"/>
+      <c r="H45" t="s">
+        <v>84</v>
+      </c>
+      <c r="I45" t="s">
+        <v>190</v>
+      </c>
+      <c r="J45"/>
+      <c r="L45" t="s">
+        <v>254</v>
+      </c>
+      <c r="M45" t="s">
+        <v>265</v>
+      </c>
+      <c r="N45" t="s">
+        <v>374</v>
+      </c>
+      <c r="O45">
+        <v>9</v>
+      </c>
+      <c r="P45" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B46" s="23" t="s">
+        <v>275</v>
+      </c>
+      <c r="C46" s="23" t="s">
+        <v>443</v>
+      </c>
+      <c r="D46" s="23" t="s">
+        <v>444</v>
+      </c>
+      <c r="E46" s="23">
+        <v>13</v>
+      </c>
+      <c r="F46" s="24" t="str">
+        <f>H44</f>
+        <v>GTIN</v>
+      </c>
+      <c r="H46" t="s">
+        <v>87</v>
+      </c>
+      <c r="I46" t="s">
+        <v>193</v>
+      </c>
+      <c r="J46" t="s">
+        <v>438</v>
+      </c>
+      <c r="L46" t="s">
+        <v>254</v>
+      </c>
+      <c r="M46" t="s">
+        <v>266</v>
+      </c>
+      <c r="N46" t="s">
+        <v>375</v>
+      </c>
+      <c r="O46">
+        <v>8</v>
+      </c>
+      <c r="P46" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>321</v>
+      </c>
+      <c r="C47" t="s">
+        <v>82</v>
+      </c>
+      <c r="D47" t="s">
+        <v>188</v>
+      </c>
+      <c r="E47">
+        <v>6</v>
+      </c>
+      <c r="F47" t="str">
+        <f>H43</f>
+        <v>LineNumber</v>
+      </c>
+      <c r="H47" t="s">
+        <v>89</v>
+      </c>
+      <c r="I47" t="s">
+        <v>195</v>
+      </c>
+      <c r="J47"/>
+      <c r="L47" t="s">
+        <v>254</v>
+      </c>
+      <c r="M47" t="s">
+        <v>267</v>
+      </c>
+      <c r="N47" t="s">
+        <v>376</v>
+      </c>
+      <c r="O47">
+        <v>13</v>
+      </c>
+      <c r="P47" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>321</v>
+      </c>
+      <c r="C48" t="s">
+        <v>85</v>
+      </c>
+      <c r="D48" t="s">
+        <v>191</v>
+      </c>
+      <c r="E48">
+        <v>13</v>
+      </c>
+      <c r="F48" t="str">
+        <f>H44</f>
+        <v>GTIN</v>
+      </c>
+      <c r="H48" t="s">
+        <v>439</v>
+      </c>
+      <c r="I48" t="s">
+        <v>440</v>
+      </c>
+      <c r="J48"/>
+      <c r="L48" t="s">
+        <v>254</v>
+      </c>
+      <c r="M48" t="s">
+        <v>268</v>
+      </c>
+      <c r="N48" t="s">
+        <v>377</v>
+      </c>
+      <c r="O48">
+        <v>1</v>
+      </c>
+      <c r="P48" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="49" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>321</v>
+      </c>
+      <c r="C49" t="s">
+        <v>84</v>
+      </c>
+      <c r="D49" t="s">
+        <v>190</v>
+      </c>
+      <c r="E49">
+        <v>35</v>
+      </c>
+      <c r="F49" t="str">
+        <f>H45</f>
+        <v>ArticleCodeSupplier</v>
+      </c>
+      <c r="H49" t="s">
+        <v>90</v>
+      </c>
+      <c r="I49" t="s">
+        <v>196</v>
+      </c>
+      <c r="J49"/>
+      <c r="L49" t="s">
+        <v>254</v>
+      </c>
+      <c r="M49" t="s">
+        <v>269</v>
+      </c>
+      <c r="N49" t="s">
+        <v>351</v>
+      </c>
+      <c r="O49">
+        <v>35</v>
+      </c>
+      <c r="P49" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="50" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>321</v>
+      </c>
+      <c r="C50" t="s">
+        <v>87</v>
+      </c>
+      <c r="D50" t="s">
+        <v>193</v>
+      </c>
+      <c r="E50">
+        <v>10</v>
+      </c>
+      <c r="F50" t="str">
+        <f>H46</f>
+        <v>OrderedQuantity</v>
+      </c>
+      <c r="H50" t="s">
+        <v>91</v>
+      </c>
+      <c r="I50" t="s">
+        <v>197</v>
+      </c>
+      <c r="J50"/>
+      <c r="L50" t="s">
+        <v>254</v>
+      </c>
+      <c r="M50" t="s">
+        <v>270</v>
+      </c>
+      <c r="N50" t="s">
+        <v>378</v>
+      </c>
+      <c r="O50">
+        <v>3</v>
+      </c>
+      <c r="P50" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="51" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>321</v>
+      </c>
+      <c r="C51" t="s">
+        <v>89</v>
+      </c>
+      <c r="D51" t="s">
+        <v>195</v>
+      </c>
+      <c r="E51">
+        <v>38</v>
+      </c>
+      <c r="F51" t="str">
+        <f>H47</f>
+        <v>ColourCode</v>
+      </c>
+      <c r="H51" t="s">
+        <v>92</v>
+      </c>
+      <c r="I51" t="s">
+        <v>198</v>
+      </c>
+      <c r="J51"/>
+      <c r="L51" t="s">
+        <v>254</v>
+      </c>
+      <c r="M51" t="s">
+        <v>271</v>
+      </c>
+      <c r="N51" t="s">
+        <v>379</v>
+      </c>
+      <c r="O51">
+        <v>35</v>
+      </c>
+      <c r="P51" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="52" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>321</v>
+      </c>
+      <c r="C52" t="s">
+        <v>439</v>
+      </c>
+      <c r="D52" t="s">
+        <v>440</v>
+      </c>
+      <c r="E52">
+        <v>20</v>
+      </c>
+      <c r="F52" t="str">
+        <f>H48</f>
+        <v>ColourSystem</v>
+      </c>
+      <c r="H52" t="s">
+        <v>93</v>
+      </c>
+      <c r="I52" t="s">
+        <v>199</v>
+      </c>
+      <c r="J52"/>
+      <c r="L52" t="s">
+        <v>254</v>
+      </c>
+      <c r="M52" t="s">
+        <v>272</v>
+      </c>
+      <c r="N52" t="s">
+        <v>380</v>
+      </c>
+      <c r="O52">
+        <v>35</v>
+      </c>
+      <c r="P52" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="53" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>321</v>
+      </c>
+      <c r="C53" t="s">
+        <v>90</v>
+      </c>
+      <c r="D53" t="s">
+        <v>196</v>
+      </c>
+      <c r="E53">
+        <v>20</v>
+      </c>
+      <c r="F53" t="str">
+        <f>H49</f>
+        <v>Length</v>
+      </c>
+      <c r="H53" t="s">
+        <v>94</v>
+      </c>
+      <c r="I53" t="s">
+        <v>200</v>
+      </c>
+      <c r="J53"/>
+      <c r="L53" t="s">
+        <v>254</v>
+      </c>
+      <c r="M53" t="s">
+        <v>273</v>
+      </c>
+      <c r="N53" t="s">
+        <v>381</v>
+      </c>
+      <c r="O53">
+        <v>35</v>
+      </c>
+      <c r="P53" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="54" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>321</v>
+      </c>
+      <c r="C54" t="s">
+        <v>91</v>
+      </c>
+      <c r="D54" t="s">
+        <v>197</v>
+      </c>
+      <c r="E54">
+        <v>4</v>
+      </c>
+      <c r="F54" t="str">
+        <f>H50</f>
+        <v>LengthUnitCode</v>
+      </c>
+      <c r="H54" t="s">
+        <v>95</v>
+      </c>
+      <c r="I54" t="s">
+        <v>201</v>
+      </c>
+      <c r="J54"/>
+      <c r="L54" t="s">
+        <v>254</v>
+      </c>
+      <c r="M54" t="s">
+        <v>274</v>
+      </c>
+      <c r="N54" t="s">
+        <v>125</v>
+      </c>
+      <c r="O54">
+        <v>8</v>
+      </c>
+      <c r="P54">
+        <f>R10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>321</v>
+      </c>
+      <c r="C55" t="s">
+        <v>92</v>
+      </c>
+      <c r="D55" t="s">
+        <v>198</v>
+      </c>
+      <c r="E55">
+        <v>20</v>
+      </c>
+      <c r="F55" t="str">
+        <f>H51</f>
+        <v>Width</v>
+      </c>
+      <c r="H55" t="s">
+        <v>96</v>
+      </c>
+      <c r="I55" t="s">
+        <v>202</v>
+      </c>
+      <c r="J55" t="s">
+        <v>438</v>
+      </c>
+      <c r="L55" t="s">
+        <v>275</v>
+      </c>
+      <c r="M55" t="s">
+        <v>276</v>
+      </c>
+      <c r="N55" t="s">
+        <v>382</v>
+      </c>
+      <c r="O55">
+        <v>13</v>
+      </c>
+      <c r="P55" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="56" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>321</v>
+      </c>
+      <c r="C56" t="s">
+        <v>93</v>
+      </c>
+      <c r="D56" t="s">
+        <v>199</v>
+      </c>
+      <c r="E56">
+        <v>4</v>
+      </c>
+      <c r="F56" t="str">
+        <f>H52</f>
+        <v>WidthUnitCode</v>
+      </c>
+      <c r="L56" t="s">
+        <v>277</v>
+      </c>
+      <c r="M56" t="s">
+        <v>278</v>
+      </c>
+      <c r="N56" t="s">
+        <v>354</v>
+      </c>
+      <c r="O56">
+        <v>35</v>
+      </c>
+      <c r="P56">
+        <f>R9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>321</v>
+      </c>
+      <c r="C57" t="s">
+        <v>94</v>
+      </c>
+      <c r="D57" t="s">
+        <v>200</v>
+      </c>
+      <c r="E57">
+        <v>20</v>
+      </c>
+      <c r="F57" t="str">
+        <f>H53</f>
+        <v>Height</v>
+      </c>
+      <c r="L57" t="s">
+        <v>277</v>
+      </c>
+      <c r="M57" t="s">
+        <v>279</v>
+      </c>
+      <c r="N57" t="s">
+        <v>383</v>
+      </c>
+      <c r="O57">
+        <v>10</v>
+      </c>
+      <c r="P57">
+        <f>R10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>321</v>
+      </c>
+      <c r="C58" t="s">
+        <v>95</v>
+      </c>
+      <c r="D58" t="s">
+        <v>201</v>
+      </c>
+      <c r="E58">
+        <v>4</v>
+      </c>
+      <c r="F58" t="str">
+        <f>H54</f>
+        <v>HeightUnitCode</v>
+      </c>
+      <c r="L58" t="s">
+        <v>277</v>
+      </c>
+      <c r="M58" t="s">
+        <v>280</v>
+      </c>
+      <c r="N58" t="s">
+        <v>128</v>
+      </c>
+      <c r="O58">
+        <v>10</v>
+      </c>
+      <c r="P58">
+        <f>R13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>321</v>
+      </c>
+      <c r="C59" t="s">
+        <v>96</v>
+      </c>
+      <c r="D59" t="s">
+        <v>202</v>
+      </c>
+      <c r="E59">
+        <v>12</v>
+      </c>
+      <c r="F59" t="str">
+        <f>H55</f>
+        <v>RetailPrice</v>
+      </c>
+      <c r="L59" t="s">
+        <v>277</v>
+      </c>
+      <c r="M59" t="s">
+        <v>281</v>
+      </c>
+      <c r="N59" t="s">
+        <v>127</v>
+      </c>
+      <c r="O59">
+        <v>10</v>
+      </c>
+      <c r="P59">
+        <f>R15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="L60" t="s">
+        <v>277</v>
+      </c>
+      <c r="M60" t="s">
+        <v>282</v>
+      </c>
+      <c r="N60" t="s">
+        <v>126</v>
+      </c>
+      <c r="O60">
+        <v>10</v>
+      </c>
+      <c r="P60">
+        <f>R14</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="L61" t="s">
+        <v>277</v>
+      </c>
+      <c r="M61" t="s">
+        <v>283</v>
+      </c>
+      <c r="N61" t="s">
+        <v>384</v>
+      </c>
+      <c r="O61">
+        <v>10</v>
+      </c>
+      <c r="P61" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="62" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="L62" t="s">
+        <v>277</v>
+      </c>
+      <c r="M62" t="s">
+        <v>284</v>
+      </c>
+      <c r="N62" t="s">
+        <v>385</v>
+      </c>
+      <c r="O62">
+        <v>3</v>
+      </c>
+      <c r="P62" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="63" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="L63" t="s">
+        <v>277</v>
+      </c>
+      <c r="M63" t="s">
+        <v>285</v>
+      </c>
+      <c r="N63" t="s">
+        <v>386</v>
+      </c>
+      <c r="O63">
+        <v>3</v>
+      </c>
+      <c r="P63" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="64" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="L64" t="s">
+        <v>277</v>
+      </c>
+      <c r="M64" t="s">
+        <v>286</v>
+      </c>
+      <c r="N64" t="s">
+        <v>387</v>
+      </c>
+      <c r="O64">
+        <v>20</v>
+      </c>
+      <c r="P64" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="65" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L65" t="s">
+        <v>277</v>
+      </c>
+      <c r="M65" t="s">
+        <v>287</v>
+      </c>
+      <c r="N65" t="s">
+        <v>388</v>
+      </c>
+      <c r="O65">
+        <v>3</v>
+      </c>
+      <c r="P65" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="66" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L66" t="s">
+        <v>277</v>
+      </c>
+      <c r="M66" t="s">
+        <v>288</v>
+      </c>
+      <c r="N66" t="s">
+        <v>389</v>
+      </c>
+      <c r="O66">
+        <v>20</v>
+      </c>
+      <c r="P66" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="67" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L67" t="s">
+        <v>277</v>
+      </c>
+      <c r="M67" t="s">
+        <v>289</v>
+      </c>
+      <c r="N67" t="s">
+        <v>390</v>
+      </c>
+      <c r="O67">
+        <v>3</v>
+      </c>
+      <c r="P67" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="68" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L68" t="s">
+        <v>277</v>
+      </c>
+      <c r="M68" t="s">
+        <v>290</v>
+      </c>
+      <c r="N68" t="s">
+        <v>391</v>
+      </c>
+      <c r="O68">
+        <v>20</v>
+      </c>
+      <c r="P68" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="69" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L69" t="s">
+        <v>277</v>
+      </c>
+      <c r="M69" t="s">
+        <v>291</v>
+      </c>
+      <c r="N69" t="s">
+        <v>392</v>
+      </c>
+      <c r="O69">
+        <v>1</v>
+      </c>
+      <c r="P69">
+        <f>R16</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L70" t="s">
+        <v>277</v>
+      </c>
+      <c r="M70" t="s">
+        <v>292</v>
+      </c>
+      <c r="N70" t="s">
+        <v>393</v>
+      </c>
+      <c r="O70">
+        <v>1</v>
+      </c>
+      <c r="P70" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="71" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L71" t="s">
+        <v>277</v>
+      </c>
+      <c r="M71" t="s">
+        <v>293</v>
+      </c>
+      <c r="N71" t="s">
+        <v>394</v>
+      </c>
+      <c r="O71">
+        <v>1</v>
+      </c>
+      <c r="P71" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="72" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L72" t="s">
+        <v>277</v>
+      </c>
+      <c r="M72" t="s">
+        <v>294</v>
+      </c>
+      <c r="N72" t="s">
+        <v>395</v>
+      </c>
+      <c r="O72">
+        <v>1</v>
+      </c>
+      <c r="P72" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="73" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L73" t="s">
+        <v>277</v>
+      </c>
+      <c r="M73" t="s">
+        <v>295</v>
+      </c>
+      <c r="N73" t="s">
+        <v>114</v>
+      </c>
+      <c r="O73">
+        <v>1</v>
+      </c>
+      <c r="P73">
+        <f>R11</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L74" t="s">
+        <v>277</v>
+      </c>
+      <c r="M74" t="s">
+        <v>296</v>
+      </c>
+      <c r="N74" t="s">
+        <v>396</v>
+      </c>
+      <c r="O74">
+        <v>1</v>
+      </c>
+      <c r="P74" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="75" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L75" t="s">
+        <v>277</v>
+      </c>
+      <c r="M75" t="s">
+        <v>297</v>
+      </c>
+      <c r="N75" t="s">
+        <v>397</v>
+      </c>
+      <c r="O75">
+        <v>1</v>
+      </c>
+      <c r="P75" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="76" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L76" t="s">
+        <v>277</v>
+      </c>
+      <c r="M76" t="s">
+        <v>298</v>
+      </c>
+      <c r="N76" t="s">
+        <v>366</v>
+      </c>
+      <c r="O76">
+        <v>1</v>
+      </c>
+      <c r="P76" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="77" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L77" t="s">
+        <v>277</v>
+      </c>
+      <c r="M77" t="s">
+        <v>299</v>
+      </c>
+      <c r="N77" t="s">
+        <v>398</v>
+      </c>
+      <c r="O77">
+        <v>1</v>
+      </c>
+      <c r="P77">
+        <f>R40</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L78" t="s">
+        <v>277</v>
+      </c>
+      <c r="M78" t="s">
+        <v>300</v>
+      </c>
+      <c r="N78" t="s">
+        <v>399</v>
+      </c>
+      <c r="O78">
+        <v>1</v>
+      </c>
+      <c r="P78">
+        <f>R41</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L79" t="s">
+        <v>277</v>
+      </c>
+      <c r="M79" t="s">
+        <v>301</v>
+      </c>
+      <c r="N79" t="s">
+        <v>400</v>
+      </c>
+      <c r="O79">
+        <v>1</v>
+      </c>
+      <c r="P79" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="80" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L80" t="s">
+        <v>277</v>
+      </c>
+      <c r="M80" t="s">
+        <v>302</v>
+      </c>
+      <c r="N80" t="s">
+        <v>401</v>
+      </c>
+      <c r="O80">
+        <v>70</v>
+      </c>
+      <c r="P80" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="81" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L81" t="s">
+        <v>277</v>
+      </c>
+      <c r="M81" t="s">
+        <v>246</v>
+      </c>
+      <c r="N81" t="s">
+        <v>358</v>
+      </c>
+      <c r="O81">
+        <v>13</v>
+      </c>
+      <c r="P81" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="82" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L82" t="s">
+        <v>277</v>
+      </c>
+      <c r="M82" t="s">
+        <v>303</v>
+      </c>
+      <c r="N82" t="s">
+        <v>402</v>
+      </c>
+      <c r="O82">
+        <v>14</v>
+      </c>
+      <c r="P82" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="83" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L83" t="s">
+        <v>277</v>
+      </c>
+      <c r="M83" t="s">
+        <v>304</v>
+      </c>
+      <c r="N83" t="s">
+        <v>403</v>
+      </c>
+      <c r="O83">
+        <v>13</v>
+      </c>
+      <c r="P83" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="84" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L84" t="s">
+        <v>277</v>
+      </c>
+      <c r="M84" t="s">
+        <v>305</v>
+      </c>
+      <c r="N84" t="s">
+        <v>404</v>
+      </c>
+      <c r="O84">
+        <v>13</v>
+      </c>
+      <c r="P84" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="85" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L85" t="s">
+        <v>277</v>
+      </c>
+      <c r="M85" t="s">
+        <v>306</v>
+      </c>
+      <c r="N85" t="s">
+        <v>405</v>
+      </c>
+      <c r="O85">
+        <v>13</v>
+      </c>
+      <c r="P85" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="86" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L86" t="s">
+        <v>277</v>
+      </c>
+      <c r="M86" t="s">
+        <v>307</v>
+      </c>
+      <c r="N86" t="s">
+        <v>406</v>
+      </c>
+      <c r="O86">
+        <v>13</v>
+      </c>
+      <c r="P86" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="87" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L87" t="s">
+        <v>277</v>
+      </c>
+      <c r="M87" t="s">
+        <v>308</v>
+      </c>
+      <c r="N87" t="s">
+        <v>360</v>
+      </c>
+      <c r="O87">
+        <v>13</v>
+      </c>
+      <c r="P87" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="88" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L88" t="s">
+        <v>277</v>
+      </c>
+      <c r="M88" t="s">
+        <v>309</v>
+      </c>
+      <c r="N88" t="s">
+        <v>407</v>
+      </c>
+      <c r="O88">
+        <v>13</v>
+      </c>
+      <c r="P88">
+        <f>R23</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L89" t="s">
+        <v>277</v>
+      </c>
+      <c r="M89" t="s">
+        <v>310</v>
+      </c>
+      <c r="N89" t="s">
+        <v>408</v>
+      </c>
+      <c r="O89">
+        <v>13</v>
+      </c>
+      <c r="P89">
+        <f>R35</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L90" t="s">
+        <v>277</v>
+      </c>
+      <c r="M90" t="s">
+        <v>311</v>
+      </c>
+      <c r="N90" t="s">
+        <v>409</v>
+      </c>
+      <c r="O90">
+        <v>13</v>
+      </c>
+      <c r="P90" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="91" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L91" t="s">
+        <v>277</v>
+      </c>
+      <c r="M91" t="s">
+        <v>312</v>
+      </c>
+      <c r="N91" t="s">
+        <v>122</v>
+      </c>
+      <c r="O91">
+        <v>35</v>
+      </c>
+      <c r="P91">
+        <f>R17</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L92" t="s">
+        <v>277</v>
+      </c>
+      <c r="M92" t="s">
+        <v>313</v>
+      </c>
+      <c r="N92" t="s">
+        <v>410</v>
+      </c>
+      <c r="O92">
+        <v>35</v>
+      </c>
+      <c r="P92" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="93" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L93" t="s">
+        <v>277</v>
+      </c>
+      <c r="M93" t="s">
+        <v>314</v>
+      </c>
+      <c r="N93" t="s">
+        <v>123</v>
+      </c>
+      <c r="O93">
+        <v>35</v>
+      </c>
+      <c r="P93" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="94" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L94" t="s">
+        <v>277</v>
+      </c>
+      <c r="M94" t="s">
+        <v>315</v>
+      </c>
+      <c r="N94" t="s">
+        <v>411</v>
+      </c>
+      <c r="O94">
+        <v>35</v>
+      </c>
+      <c r="P94" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="95" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L95" t="s">
+        <v>277</v>
+      </c>
+      <c r="M95" t="s">
+        <v>316</v>
+      </c>
+      <c r="N95" t="s">
+        <v>412</v>
+      </c>
+      <c r="O95">
+        <v>1</v>
+      </c>
+      <c r="P95">
+        <f>R7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L96" t="s">
+        <v>277</v>
+      </c>
+      <c r="M96" t="s">
+        <v>317</v>
+      </c>
+      <c r="N96" t="s">
+        <v>413</v>
+      </c>
+      <c r="O96">
+        <v>5</v>
+      </c>
+      <c r="P96">
+        <f>R17</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L97" t="s">
+        <v>277</v>
+      </c>
+      <c r="M97" t="s">
+        <v>318</v>
+      </c>
+      <c r="N97" t="s">
+        <v>414</v>
+      </c>
+      <c r="O97">
+        <v>5</v>
+      </c>
+      <c r="P97">
+        <f>R13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L98" t="s">
+        <v>277</v>
+      </c>
+      <c r="M98" t="s">
+        <v>319</v>
+      </c>
+      <c r="N98" t="s">
+        <v>415</v>
+      </c>
+      <c r="O98">
+        <v>5</v>
+      </c>
+      <c r="P98">
+        <f>R19</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L99" t="s">
+        <v>277</v>
+      </c>
+      <c r="M99" t="s">
+        <v>320</v>
+      </c>
+      <c r="N99" t="s">
+        <v>416</v>
+      </c>
+      <c r="O99">
+        <v>5</v>
+      </c>
+      <c r="P99">
+        <f>R16</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L100" s="9" t="s">
+        <v>427</v>
+      </c>
+      <c r="M100" s="10"/>
+      <c r="N100" s="10"/>
+      <c r="O100" s="13"/>
+      <c r="P100" s="10"/>
+    </row>
+    <row r="101" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L101" t="s">
+        <v>321</v>
+      </c>
+      <c r="M101" t="s">
+        <v>325</v>
+      </c>
+      <c r="N101" t="s">
+        <v>418</v>
+      </c>
+      <c r="O101">
+        <v>14</v>
+      </c>
+      <c r="P101">
+        <f>R44</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L102" t="s">
+        <v>321</v>
+      </c>
+      <c r="M102" t="s">
+        <v>330</v>
+      </c>
+      <c r="N102" t="s">
+        <v>422</v>
+      </c>
+      <c r="O102">
+        <v>35</v>
+      </c>
+      <c r="P102" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="103" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L103" t="s">
+        <v>321</v>
+      </c>
+      <c r="M103" t="s">
+        <v>324</v>
+      </c>
+      <c r="N103" t="s">
+        <v>189</v>
+      </c>
+      <c r="O103">
+        <v>35</v>
+      </c>
+      <c r="P103" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="104" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L104" t="s">
+        <v>321</v>
+      </c>
+      <c r="M104" t="s">
+        <v>328</v>
+      </c>
+      <c r="N104" t="s">
+        <v>420</v>
+      </c>
+      <c r="O104">
+        <v>38</v>
+      </c>
+      <c r="P104" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="105" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L105" t="s">
+        <v>321</v>
+      </c>
+      <c r="M105" t="s">
+        <v>329</v>
+      </c>
+      <c r="N105" t="s">
+        <v>421</v>
+      </c>
+      <c r="O105">
+        <v>20</v>
+      </c>
+      <c r="P105" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="106" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L106" t="s">
+        <v>321</v>
+      </c>
+      <c r="M106" t="s">
+        <v>322</v>
+      </c>
+      <c r="N106" t="s">
+        <v>417</v>
+      </c>
+      <c r="O106">
+        <v>20</v>
+      </c>
+      <c r="P106" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="107" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L107" t="s">
+        <v>321</v>
+      </c>
+      <c r="M107" t="s">
+        <v>327</v>
+      </c>
+      <c r="N107" t="s">
+        <v>419</v>
+      </c>
+      <c r="O107">
+        <v>20</v>
+      </c>
+      <c r="P107" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="108" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L108" t="s">
+        <v>321</v>
+      </c>
+      <c r="M108" t="s">
+        <v>323</v>
+      </c>
+      <c r="N108" t="s">
+        <v>159</v>
+      </c>
+      <c r="O108">
+        <v>3</v>
+      </c>
+      <c r="P108" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="109" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L109" t="s">
+        <v>321</v>
+      </c>
+      <c r="M109" t="s">
+        <v>332</v>
+      </c>
+      <c r="N109" t="s">
+        <v>357</v>
+      </c>
+      <c r="O109">
+        <v>10</v>
+      </c>
+      <c r="P109" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="110" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L110" t="s">
+        <v>321</v>
+      </c>
+      <c r="M110" t="s">
+        <v>334</v>
+      </c>
+      <c r="N110" t="s">
+        <v>424</v>
+      </c>
+      <c r="O110">
+        <v>35</v>
+      </c>
+      <c r="P110" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="111" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L111" t="s">
+        <v>321</v>
+      </c>
+      <c r="M111" t="s">
+        <v>335</v>
+      </c>
+      <c r="N111" t="s">
+        <v>425</v>
+      </c>
+      <c r="O111">
+        <v>10</v>
+      </c>
+      <c r="P111" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="112" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L112" t="s">
+        <v>277</v>
+      </c>
+      <c r="M112" t="s">
+        <v>225</v>
+      </c>
+      <c r="N112" t="s">
+        <v>340</v>
+      </c>
+      <c r="O112">
+        <v>8</v>
+      </c>
+      <c r="P112" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="113" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L113" t="s">
+        <v>321</v>
+      </c>
+      <c r="M113" t="s">
+        <v>331</v>
+      </c>
+      <c r="N113" t="s">
+        <v>188</v>
+      </c>
+      <c r="O113">
+        <v>6</v>
+      </c>
+      <c r="P113">
+        <f>R43</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L114" t="s">
+        <v>321</v>
+      </c>
+      <c r="M114" t="s">
+        <v>333</v>
+      </c>
+      <c r="N114" t="s">
+        <v>423</v>
+      </c>
+      <c r="O114">
+        <v>12</v>
+      </c>
+      <c r="P114" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="115" spans="12:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="L115" t="s">
         <v>321</v>
       </c>

</xml_diff>

<commit_message>
[CHANGE] Removed TrusedUser. Used CodeBars in select query to find article. Check if UDF file exists before loading the UDF xml file
</commit_message>
<xml_diff>
--- a/TransusFieldsMapping.xlsx
+++ b/TransusFieldsMapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Order Plastica v2" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2149" uniqueCount="451">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2149" uniqueCount="453">
   <si>
     <t>Table</t>
   </si>
@@ -1369,13 +1369,19 @@
   </si>
   <si>
     <t>GLN van de partner</t>
+  </si>
+  <si>
+    <t>CodeBars</t>
+  </si>
+  <si>
+    <t>SAP Field</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1435,8 +1441,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1468,6 +1481,11 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -1513,15 +1531,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1560,6 +1579,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1575,14 +1596,14 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="6"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="40% - Accent4" xfId="4" builtinId="43"/>
     <cellStyle name="40% - Accent6" xfId="5" builtinId="51"/>
     <cellStyle name="Accent1" xfId="3" builtinId="29"/>
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Good" xfId="6" builtinId="26"/>
     <cellStyle name="Input" xfId="2" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -2228,6 +2249,13 @@
       </border>
     </dxf>
     <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
@@ -2436,13 +2464,6 @@
         <right/>
         <top/>
         <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -2689,11 +2710,11 @@
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table3713" displayName="Table3713" ref="L101:P115" headerRowCount="0" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
   <tableColumns count="5">
-    <tableColumn id="1" name="Column1" headerRowDxfId="35" dataCellStyle="Normal"/>
-    <tableColumn id="2" name="Column2" headerRowDxfId="34" dataCellStyle="Normal"/>
-    <tableColumn id="3" name="Column3" headerRowDxfId="33" dataCellStyle="Normal"/>
-    <tableColumn id="4" name="Column4" headerRowDxfId="32" dataCellStyle="Normal"/>
-    <tableColumn id="5" name="Column5" headerRowDxfId="31" dataCellStyle="Normal"/>
+    <tableColumn id="1" name="Column1" headerRowDxfId="25" dataCellStyle="Normal"/>
+    <tableColumn id="2" name="Column2" headerRowDxfId="24" dataCellStyle="Normal"/>
+    <tableColumn id="3" name="Column3" headerRowDxfId="23" dataCellStyle="Normal"/>
+    <tableColumn id="4" name="Column4" headerRowDxfId="22" dataCellStyle="Normal"/>
+    <tableColumn id="5" name="Column5" headerRowDxfId="21" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2811,11 +2832,11 @@
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table22" displayName="Table22" ref="B5:F44" headerRowCount="0" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
   <tableColumns count="5">
-    <tableColumn id="1" name="Column1" headerRowDxfId="30" dataCellStyle="Normal"/>
-    <tableColumn id="2" name="Column2" headerRowDxfId="29" dataCellStyle="Normal"/>
-    <tableColumn id="3" name="Column3" headerRowDxfId="28" dataCellStyle="Normal"/>
-    <tableColumn id="4" name="Column4" headerRowDxfId="27" dataCellStyle="Normal"/>
-    <tableColumn id="5" name="Column5" headerRowDxfId="26" dataCellStyle="Normal"/>
+    <tableColumn id="1" name="Column1" headerRowDxfId="41" dataCellStyle="Normal"/>
+    <tableColumn id="2" name="Column2" headerRowDxfId="40" dataCellStyle="Normal"/>
+    <tableColumn id="3" name="Column3" headerRowDxfId="39" dataCellStyle="Normal"/>
+    <tableColumn id="4" name="Column4" headerRowDxfId="38" dataCellStyle="Normal"/>
+    <tableColumn id="5" name="Column5" headerRowDxfId="37" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2824,11 +2845,11 @@
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table37" displayName="Table37" ref="B46:F59" headerRowCount="0" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
   <tableColumns count="5">
-    <tableColumn id="1" name="Column1" headerRowDxfId="25" dataCellStyle="Normal"/>
-    <tableColumn id="2" name="Column2" headerRowDxfId="24" dataCellStyle="Normal"/>
-    <tableColumn id="3" name="Column3" headerRowDxfId="23" dataCellStyle="Normal"/>
-    <tableColumn id="4" name="Column4" headerRowDxfId="22" dataCellStyle="Normal"/>
-    <tableColumn id="5" name="Column5" headerRowDxfId="21" dataCellStyle="Normal"/>
+    <tableColumn id="1" name="Column1" headerRowDxfId="36" dataCellStyle="Normal"/>
+    <tableColumn id="2" name="Column2" headerRowDxfId="35" dataCellStyle="Normal"/>
+    <tableColumn id="3" name="Column3" headerRowDxfId="34" dataCellStyle="Normal"/>
+    <tableColumn id="4" name="Column4" headerRowDxfId="33" dataCellStyle="Normal"/>
+    <tableColumn id="5" name="Column5" headerRowDxfId="32" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2846,7 +2867,7 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table59" displayName="Table59" ref="H5:J41" headerRowCount="0" totalsRowShown="0" tableBorderDxfId="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table59" displayName="Table59" ref="H5:J41" headerRowCount="0" totalsRowShown="0" tableBorderDxfId="31">
   <tableColumns count="3">
     <tableColumn id="1" name="Column1"/>
     <tableColumn id="2" name="Column2"/>
@@ -2859,11 +2880,11 @@
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table2212" displayName="Table2212" ref="L5:P99" headerRowCount="0" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
   <tableColumns count="5">
-    <tableColumn id="1" name="Column1" headerRowDxfId="40" dataCellStyle="Normal"/>
-    <tableColumn id="2" name="Column2" headerRowDxfId="39" dataCellStyle="Normal"/>
-    <tableColumn id="3" name="Column3" headerRowDxfId="38" dataCellStyle="Normal"/>
-    <tableColumn id="4" name="Column4" headerRowDxfId="37" dataCellStyle="Normal"/>
-    <tableColumn id="5" name="Column5" headerRowDxfId="36" dataCellStyle="Normal"/>
+    <tableColumn id="1" name="Column1" headerRowDxfId="30" dataCellStyle="Normal"/>
+    <tableColumn id="2" name="Column2" headerRowDxfId="29" dataCellStyle="Normal"/>
+    <tableColumn id="3" name="Column3" headerRowDxfId="28" dataCellStyle="Normal"/>
+    <tableColumn id="4" name="Column4" headerRowDxfId="27" dataCellStyle="Normal"/>
+    <tableColumn id="5" name="Column5" headerRowDxfId="26" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3191,24 +3212,24 @@
       <c r="J1" s="7"/>
     </row>
     <row r="2" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="22" t="s">
         <v>430</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="23" t="s">
         <v>431</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="H2" s="18" t="s">
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="H2" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
     </row>
     <row r="3" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="20"/>
+      <c r="A3" s="22"/>
       <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
@@ -6184,8 +6205,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P115"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6229,31 +6250,31 @@
       <c r="P1" s="6"/>
     </row>
     <row r="2" spans="1:16" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="22" t="s">
         <v>430</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="23" t="s">
         <v>431</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="H2" s="18" t="s">
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="H2" s="20" t="s">
         <v>433</v>
       </c>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="L2" s="21" t="s">
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="L2" s="23" t="s">
         <v>431</v>
       </c>
-      <c r="M2" s="22"/>
-      <c r="N2" s="22"/>
-      <c r="O2" s="22"/>
-      <c r="P2" s="22"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="24"/>
+      <c r="O2" s="24"/>
+      <c r="P2" s="24"/>
     </row>
     <row r="3" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="20"/>
+      <c r="A3" s="22"/>
       <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
@@ -7813,19 +7834,19 @@
       <c r="A42" t="s">
         <v>448</v>
       </c>
-      <c r="B42" s="23" t="s">
+      <c r="B42" s="18" t="s">
         <v>441</v>
       </c>
-      <c r="C42" s="23" t="s">
+      <c r="C42" s="18" t="s">
         <v>447</v>
       </c>
-      <c r="D42" s="23" t="s">
+      <c r="D42" s="18" t="s">
         <v>446</v>
       </c>
-      <c r="E42" s="23">
+      <c r="E42" s="18">
         <v>13</v>
       </c>
-      <c r="F42" s="24" t="str">
+      <c r="F42" s="19" t="str">
         <f>H26</f>
         <v>InvoiceeGLN</v>
       </c>
@@ -7854,19 +7875,19 @@
       <c r="A43" t="s">
         <v>449</v>
       </c>
-      <c r="B43" s="23" t="s">
+      <c r="B43" s="18" t="s">
         <v>441</v>
       </c>
-      <c r="C43" s="23" t="s">
+      <c r="C43" s="18" t="s">
         <v>447</v>
       </c>
-      <c r="D43" s="23" t="s">
+      <c r="D43" s="18" t="s">
         <v>446</v>
       </c>
-      <c r="E43" s="23">
+      <c r="E43" s="18">
         <v>13</v>
       </c>
-      <c r="F43" s="24" t="str">
+      <c r="F43" s="19" t="str">
         <f>CONCATENATE(H28, " or ", H20)</f>
         <v>DeliveryPartyGLN or BuyerGLN</v>
       </c>
@@ -7894,19 +7915,19 @@
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B44" s="23" t="s">
+      <c r="B44" s="18" t="s">
         <v>442</v>
       </c>
-      <c r="C44" s="23" t="s">
+      <c r="C44" s="18" t="s">
         <v>445</v>
       </c>
-      <c r="D44" s="23" t="s">
+      <c r="D44" s="18" t="s">
         <v>450</v>
       </c>
-      <c r="E44" s="23">
+      <c r="E44" s="18">
         <v>13</v>
       </c>
-      <c r="F44" s="24" t="str">
+      <c r="F44" s="19" t="str">
         <f>H20</f>
         <v>BuyerGLN</v>
       </c>
@@ -7965,19 +7986,19 @@
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B46" s="23" t="s">
+      <c r="B46" s="18" t="s">
         <v>275</v>
       </c>
-      <c r="C46" s="23" t="s">
-        <v>443</v>
-      </c>
-      <c r="D46" s="23" t="s">
-        <v>444</v>
-      </c>
-      <c r="E46" s="23">
+      <c r="C46" s="18" t="s">
+        <v>451</v>
+      </c>
+      <c r="D46" s="25" t="s">
+        <v>452</v>
+      </c>
+      <c r="E46" s="18">
         <v>13</v>
       </c>
-      <c r="F46" s="24" t="str">
+      <c r="F46" s="19" t="str">
         <f>H44</f>
         <v>GTIN</v>
       </c>
@@ -8020,7 +8041,7 @@
         <v>6</v>
       </c>
       <c r="F47" t="str">
-        <f>H43</f>
+        <f t="shared" ref="F47:F59" si="0">H43</f>
         <v>LineNumber</v>
       </c>
       <c r="H47" t="s">
@@ -8060,7 +8081,7 @@
         <v>13</v>
       </c>
       <c r="F48" t="str">
-        <f>H44</f>
+        <f t="shared" si="0"/>
         <v>GTIN</v>
       </c>
       <c r="H48" t="s">
@@ -8100,7 +8121,7 @@
         <v>35</v>
       </c>
       <c r="F49" t="str">
-        <f>H45</f>
+        <f t="shared" si="0"/>
         <v>ArticleCodeSupplier</v>
       </c>
       <c r="H49" t="s">
@@ -8140,7 +8161,7 @@
         <v>10</v>
       </c>
       <c r="F50" t="str">
-        <f>H46</f>
+        <f t="shared" si="0"/>
         <v>OrderedQuantity</v>
       </c>
       <c r="H50" t="s">
@@ -8180,7 +8201,7 @@
         <v>38</v>
       </c>
       <c r="F51" t="str">
-        <f>H47</f>
+        <f t="shared" si="0"/>
         <v>ColourCode</v>
       </c>
       <c r="H51" t="s">
@@ -8220,7 +8241,7 @@
         <v>20</v>
       </c>
       <c r="F52" t="str">
-        <f>H48</f>
+        <f t="shared" si="0"/>
         <v>ColourSystem</v>
       </c>
       <c r="H52" t="s">
@@ -8260,7 +8281,7 @@
         <v>20</v>
       </c>
       <c r="F53" t="str">
-        <f>H49</f>
+        <f t="shared" si="0"/>
         <v>Length</v>
       </c>
       <c r="H53" t="s">
@@ -8300,7 +8321,7 @@
         <v>4</v>
       </c>
       <c r="F54" t="str">
-        <f>H50</f>
+        <f t="shared" si="0"/>
         <v>LengthUnitCode</v>
       </c>
       <c r="H54" t="s">
@@ -8341,7 +8362,7 @@
         <v>20</v>
       </c>
       <c r="F55" t="str">
-        <f>H51</f>
+        <f t="shared" si="0"/>
         <v>Width</v>
       </c>
       <c r="H55" t="s">
@@ -8383,7 +8404,7 @@
         <v>4</v>
       </c>
       <c r="F56" t="str">
-        <f>H52</f>
+        <f t="shared" si="0"/>
         <v>WidthUnitCode</v>
       </c>
       <c r="L56" t="s">
@@ -8417,7 +8438,7 @@
         <v>20</v>
       </c>
       <c r="F57" t="str">
-        <f>H53</f>
+        <f t="shared" si="0"/>
         <v>Height</v>
       </c>
       <c r="L57" t="s">
@@ -8451,7 +8472,7 @@
         <v>4</v>
       </c>
       <c r="F58" t="str">
-        <f>H54</f>
+        <f t="shared" si="0"/>
         <v>HeightUnitCode</v>
       </c>
       <c r="L58" t="s">
@@ -8485,7 +8506,7 @@
         <v>12</v>
       </c>
       <c r="F59" t="str">
-        <f>H55</f>
+        <f t="shared" si="0"/>
         <v>RetailPrice</v>
       </c>
       <c r="L59" t="s">
@@ -9500,7 +9521,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P115"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
@@ -9545,31 +9566,31 @@
       <c r="P1" s="6"/>
     </row>
     <row r="2" spans="1:16" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="22" t="s">
         <v>430</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="23" t="s">
         <v>431</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="H2" s="18" t="s">
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="H2" s="20" t="s">
         <v>433</v>
       </c>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="L2" s="21" t="s">
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="L2" s="23" t="s">
         <v>431</v>
       </c>
-      <c r="M2" s="22"/>
-      <c r="N2" s="22"/>
-      <c r="O2" s="22"/>
-      <c r="P2" s="22"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="24"/>
+      <c r="O2" s="24"/>
+      <c r="P2" s="24"/>
     </row>
     <row r="3" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="20"/>
+      <c r="A3" s="22"/>
       <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
@@ -11129,19 +11150,19 @@
       <c r="A42" t="s">
         <v>448</v>
       </c>
-      <c r="B42" s="23" t="s">
+      <c r="B42" s="18" t="s">
         <v>441</v>
       </c>
-      <c r="C42" s="23" t="s">
+      <c r="C42" s="18" t="s">
         <v>447</v>
       </c>
-      <c r="D42" s="23" t="s">
+      <c r="D42" s="18" t="s">
         <v>446</v>
       </c>
-      <c r="E42" s="23">
+      <c r="E42" s="18">
         <v>13</v>
       </c>
-      <c r="F42" s="24" t="str">
+      <c r="F42" s="19" t="str">
         <f>H26</f>
         <v>InvoiceeGLN</v>
       </c>
@@ -11170,19 +11191,19 @@
       <c r="A43" t="s">
         <v>449</v>
       </c>
-      <c r="B43" s="23" t="s">
+      <c r="B43" s="18" t="s">
         <v>441</v>
       </c>
-      <c r="C43" s="23" t="s">
+      <c r="C43" s="18" t="s">
         <v>447</v>
       </c>
-      <c r="D43" s="23" t="s">
+      <c r="D43" s="18" t="s">
         <v>446</v>
       </c>
-      <c r="E43" s="23">
+      <c r="E43" s="18">
         <v>13</v>
       </c>
-      <c r="F43" s="24" t="str">
+      <c r="F43" s="19" t="str">
         <f>CONCATENATE(H28, " or ", H20)</f>
         <v>DeliveryPartyGLN or BuyerGLN</v>
       </c>
@@ -11210,19 +11231,19 @@
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B44" s="23" t="s">
+      <c r="B44" s="18" t="s">
         <v>442</v>
       </c>
-      <c r="C44" s="23" t="s">
+      <c r="C44" s="18" t="s">
         <v>445</v>
       </c>
-      <c r="D44" s="23" t="s">
+      <c r="D44" s="18" t="s">
         <v>450</v>
       </c>
-      <c r="E44" s="23">
+      <c r="E44" s="18">
         <v>13</v>
       </c>
-      <c r="F44" s="24" t="str">
+      <c r="F44" s="19" t="str">
         <f>H20</f>
         <v>BuyerGLN</v>
       </c>
@@ -11281,19 +11302,19 @@
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B46" s="23" t="s">
+      <c r="B46" s="18" t="s">
         <v>275</v>
       </c>
-      <c r="C46" s="23" t="s">
+      <c r="C46" s="18" t="s">
         <v>443</v>
       </c>
-      <c r="D46" s="23" t="s">
+      <c r="D46" s="18" t="s">
         <v>444</v>
       </c>
-      <c r="E46" s="23">
+      <c r="E46" s="18">
         <v>13</v>
       </c>
-      <c r="F46" s="24" t="str">
+      <c r="F46" s="19" t="str">
         <f>H44</f>
         <v>GTIN</v>
       </c>
@@ -11336,7 +11357,7 @@
         <v>6</v>
       </c>
       <c r="F47" t="str">
-        <f>H43</f>
+        <f t="shared" ref="F47:F59" si="0">H43</f>
         <v>LineNumber</v>
       </c>
       <c r="H47" t="s">
@@ -11376,7 +11397,7 @@
         <v>13</v>
       </c>
       <c r="F48" t="str">
-        <f>H44</f>
+        <f t="shared" si="0"/>
         <v>GTIN</v>
       </c>
       <c r="H48" t="s">
@@ -11416,7 +11437,7 @@
         <v>35</v>
       </c>
       <c r="F49" t="str">
-        <f>H45</f>
+        <f t="shared" si="0"/>
         <v>ArticleCodeSupplier</v>
       </c>
       <c r="H49" t="s">
@@ -11456,7 +11477,7 @@
         <v>10</v>
       </c>
       <c r="F50" t="str">
-        <f>H46</f>
+        <f t="shared" si="0"/>
         <v>OrderedQuantity</v>
       </c>
       <c r="H50" t="s">
@@ -11496,7 +11517,7 @@
         <v>38</v>
       </c>
       <c r="F51" t="str">
-        <f>H47</f>
+        <f t="shared" si="0"/>
         <v>ColourCode</v>
       </c>
       <c r="H51" t="s">
@@ -11536,7 +11557,7 @@
         <v>20</v>
       </c>
       <c r="F52" t="str">
-        <f>H48</f>
+        <f t="shared" si="0"/>
         <v>ColourSystem</v>
       </c>
       <c r="H52" t="s">
@@ -11576,7 +11597,7 @@
         <v>20</v>
       </c>
       <c r="F53" t="str">
-        <f>H49</f>
+        <f t="shared" si="0"/>
         <v>Length</v>
       </c>
       <c r="H53" t="s">
@@ -11616,7 +11637,7 @@
         <v>4</v>
       </c>
       <c r="F54" t="str">
-        <f>H50</f>
+        <f t="shared" si="0"/>
         <v>LengthUnitCode</v>
       </c>
       <c r="H54" t="s">
@@ -11657,7 +11678,7 @@
         <v>20</v>
       </c>
       <c r="F55" t="str">
-        <f>H51</f>
+        <f t="shared" si="0"/>
         <v>Width</v>
       </c>
       <c r="H55" t="s">
@@ -11699,7 +11720,7 @@
         <v>4</v>
       </c>
       <c r="F56" t="str">
-        <f>H52</f>
+        <f t="shared" si="0"/>
         <v>WidthUnitCode</v>
       </c>
       <c r="L56" t="s">
@@ -11733,7 +11754,7 @@
         <v>20</v>
       </c>
       <c r="F57" t="str">
-        <f>H53</f>
+        <f t="shared" si="0"/>
         <v>Height</v>
       </c>
       <c r="L57" t="s">
@@ -11767,7 +11788,7 @@
         <v>4</v>
       </c>
       <c r="F58" t="str">
-        <f>H54</f>
+        <f t="shared" si="0"/>
         <v>HeightUnitCode</v>
       </c>
       <c r="L58" t="s">
@@ -11801,7 +11822,7 @@
         <v>12</v>
       </c>
       <c r="F59" t="str">
-        <f>H55</f>
+        <f t="shared" si="0"/>
         <v>RetailPrice</v>
       </c>
       <c r="L59" t="s">

</xml_diff>